<commit_message>
RDCC-2480: updating test files with valid first and last names
</commit_message>
<xml_diff>
--- a/src/integrationTest/resources/Staff Data Upload With All Valid Rows.xlsx
+++ b/src/integrationTest/resources/Staff Data Upload With All Valid Rows.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_900458/Documents/HMCTS/rd-caseworker-ref-api/src/integrationTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69B0217-5F76-EE41-9EDA-1FF9D6FD2EFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0ABE6CC-E9EF-1347-B7C3-666EAAB8B8E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1680" yWindow="1800" windowWidth="23260" windowHeight="12580" activeTab="3" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
   </bookViews>
@@ -3888,7 +3888,7 @@
     <t>test-2@justice.gov.uk</t>
   </si>
   <si>
-    <t>test2</t>
+    <t>ttest</t>
   </si>
 </sst>
 </file>
@@ -4454,19 +4454,7 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -4474,12 +4462,24 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -13108,16 +13108,16 @@
     </row>
     <row r="4" spans="1:34" s="70" customFormat="1" ht="34.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="68"/>
-      <c r="B4" s="76" t="s">
+      <c r="B4" s="72" t="s">
         <v>1208</v>
       </c>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="76"/>
-      <c r="I4" s="76"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="72"/>
+      <c r="H4" s="72"/>
+      <c r="I4" s="72"/>
       <c r="J4" s="68"/>
       <c r="K4" s="68"/>
       <c r="L4" s="67" t="s">
@@ -13132,16 +13132,16 @@
       <c r="S4" s="68"/>
       <c r="T4" s="68"/>
       <c r="U4" s="68"/>
-      <c r="V4" s="76" t="s">
+      <c r="V4" s="72" t="s">
         <v>1210</v>
       </c>
-      <c r="W4" s="76"/>
-      <c r="X4" s="76"/>
-      <c r="Y4" s="76"/>
-      <c r="Z4" s="76"/>
-      <c r="AA4" s="76"/>
-      <c r="AB4" s="76"/>
-      <c r="AC4" s="76"/>
+      <c r="W4" s="72"/>
+      <c r="X4" s="72"/>
+      <c r="Y4" s="72"/>
+      <c r="Z4" s="72"/>
+      <c r="AA4" s="72"/>
+      <c r="AB4" s="72"/>
+      <c r="AC4" s="72"/>
       <c r="AD4" s="69"/>
       <c r="AE4" s="69"/>
       <c r="AF4" s="69"/>
@@ -13150,16 +13150,16 @@
     </row>
     <row r="5" spans="1:34" ht="31.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="30"/>
-      <c r="B5" s="77" t="s">
+      <c r="B5" s="73" t="s">
         <v>1235</v>
       </c>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
       <c r="J5" s="30"/>
       <c r="K5" s="30"/>
       <c r="L5" s="30"/>
@@ -13172,16 +13172,16 @@
       <c r="S5" s="30"/>
       <c r="T5" s="30"/>
       <c r="U5" s="30"/>
-      <c r="V5" s="78" t="s">
+      <c r="V5" s="75" t="s">
         <v>1211</v>
       </c>
-      <c r="W5" s="71"/>
-      <c r="X5" s="71"/>
-      <c r="Y5" s="71"/>
-      <c r="Z5" s="71"/>
-      <c r="AA5" s="71"/>
-      <c r="AB5" s="71"/>
-      <c r="AC5" s="71"/>
+      <c r="W5" s="74"/>
+      <c r="X5" s="74"/>
+      <c r="Y5" s="74"/>
+      <c r="Z5" s="74"/>
+      <c r="AA5" s="74"/>
+      <c r="AB5" s="74"/>
+      <c r="AC5" s="74"/>
     </row>
     <row r="6" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="30"/>
@@ -13216,16 +13216,16 @@
     </row>
     <row r="7" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="30"/>
-      <c r="B7" s="79" t="s">
+      <c r="B7" s="76" t="s">
         <v>1212</v>
       </c>
-      <c r="C7" s="79"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="79"/>
-      <c r="F7" s="79"/>
-      <c r="G7" s="79"/>
-      <c r="H7" s="79"/>
-      <c r="I7" s="79"/>
+      <c r="C7" s="76"/>
+      <c r="D7" s="76"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="76"/>
+      <c r="H7" s="76"/>
+      <c r="I7" s="76"/>
       <c r="J7" s="30"/>
       <c r="K7" s="30"/>
       <c r="L7" s="30"/>
@@ -13238,29 +13238,29 @@
       <c r="S7" s="30"/>
       <c r="T7" s="30"/>
       <c r="U7" s="30"/>
-      <c r="V7" s="79" t="s">
+      <c r="V7" s="76" t="s">
         <v>1213</v>
       </c>
-      <c r="W7" s="79"/>
-      <c r="X7" s="79"/>
-      <c r="Y7" s="79"/>
-      <c r="Z7" s="79"/>
-      <c r="AA7" s="79"/>
-      <c r="AB7" s="79"/>
-      <c r="AC7" s="79"/>
+      <c r="W7" s="76"/>
+      <c r="X7" s="76"/>
+      <c r="Y7" s="76"/>
+      <c r="Z7" s="76"/>
+      <c r="AA7" s="76"/>
+      <c r="AB7" s="76"/>
+      <c r="AC7" s="76"/>
     </row>
     <row r="8" spans="1:34" ht="32.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="30"/>
-      <c r="B8" s="73" t="s">
+      <c r="B8" s="77" t="s">
         <v>1214</v>
       </c>
-      <c r="C8" s="73"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73"/>
-      <c r="G8" s="73"/>
-      <c r="H8" s="73"/>
-      <c r="I8" s="73"/>
+      <c r="C8" s="77"/>
+      <c r="D8" s="77"/>
+      <c r="E8" s="77"/>
+      <c r="F8" s="77"/>
+      <c r="G8" s="77"/>
+      <c r="H8" s="77"/>
+      <c r="I8" s="77"/>
       <c r="J8" s="30"/>
       <c r="K8" s="30"/>
       <c r="L8" s="30"/>
@@ -13273,16 +13273,16 @@
       <c r="S8" s="30"/>
       <c r="T8" s="30"/>
       <c r="U8" s="30"/>
-      <c r="V8" s="73" t="s">
+      <c r="V8" s="77" t="s">
         <v>1215</v>
       </c>
-      <c r="W8" s="73"/>
-      <c r="X8" s="73"/>
-      <c r="Y8" s="73"/>
-      <c r="Z8" s="73"/>
-      <c r="AA8" s="73"/>
-      <c r="AB8" s="73"/>
-      <c r="AC8" s="73"/>
+      <c r="W8" s="77"/>
+      <c r="X8" s="77"/>
+      <c r="Y8" s="77"/>
+      <c r="Z8" s="77"/>
+      <c r="AA8" s="77"/>
+      <c r="AB8" s="77"/>
+      <c r="AC8" s="77"/>
     </row>
     <row r="9" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="30"/>
@@ -13337,16 +13337,16 @@
       <c r="S10" s="30"/>
       <c r="T10" s="30"/>
       <c r="U10" s="30"/>
-      <c r="V10" s="73" t="s">
+      <c r="V10" s="77" t="s">
         <v>1216</v>
       </c>
-      <c r="W10" s="73"/>
-      <c r="X10" s="73"/>
-      <c r="Y10" s="73"/>
-      <c r="Z10" s="73"/>
-      <c r="AA10" s="73"/>
-      <c r="AB10" s="73"/>
-      <c r="AC10" s="73"/>
+      <c r="W10" s="77"/>
+      <c r="X10" s="77"/>
+      <c r="Y10" s="77"/>
+      <c r="Z10" s="77"/>
+      <c r="AA10" s="77"/>
+      <c r="AB10" s="77"/>
+      <c r="AC10" s="77"/>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A11" s="30"/>
@@ -13515,16 +13515,16 @@
       <c r="I16" s="30"/>
       <c r="J16" s="30"/>
       <c r="K16" s="30"/>
-      <c r="L16" s="74" t="s">
+      <c r="L16" s="71" t="s">
         <v>1217</v>
       </c>
-      <c r="M16" s="74"/>
-      <c r="N16" s="74"/>
-      <c r="O16" s="74"/>
-      <c r="P16" s="74"/>
-      <c r="Q16" s="74"/>
-      <c r="R16" s="74"/>
-      <c r="S16" s="74"/>
+      <c r="M16" s="71"/>
+      <c r="N16" s="71"/>
+      <c r="O16" s="71"/>
+      <c r="P16" s="71"/>
+      <c r="Q16" s="71"/>
+      <c r="R16" s="71"/>
+      <c r="S16" s="71"/>
       <c r="T16" s="30"/>
       <c r="U16" s="30"/>
       <c r="V16" s="30"/>
@@ -13548,14 +13548,14 @@
       <c r="I17" s="30"/>
       <c r="J17" s="30"/>
       <c r="K17" s="30"/>
-      <c r="L17" s="74"/>
-      <c r="M17" s="74"/>
-      <c r="N17" s="74"/>
-      <c r="O17" s="74"/>
-      <c r="P17" s="74"/>
-      <c r="Q17" s="74"/>
-      <c r="R17" s="74"/>
-      <c r="S17" s="74"/>
+      <c r="L17" s="71"/>
+      <c r="M17" s="71"/>
+      <c r="N17" s="71"/>
+      <c r="O17" s="71"/>
+      <c r="P17" s="71"/>
+      <c r="Q17" s="71"/>
+      <c r="R17" s="71"/>
+      <c r="S17" s="71"/>
       <c r="T17" s="30"/>
       <c r="U17" s="30"/>
       <c r="V17" s="30"/>
@@ -13579,16 +13579,16 @@
       <c r="I18" s="30"/>
       <c r="J18" s="30"/>
       <c r="K18" s="30"/>
-      <c r="L18" s="80" t="s">
+      <c r="L18" s="78" t="s">
         <v>1218</v>
       </c>
-      <c r="M18" s="75"/>
-      <c r="N18" s="75"/>
-      <c r="O18" s="75"/>
-      <c r="P18" s="75"/>
-      <c r="Q18" s="75"/>
-      <c r="R18" s="75"/>
-      <c r="S18" s="75"/>
+      <c r="M18" s="79"/>
+      <c r="N18" s="79"/>
+      <c r="O18" s="79"/>
+      <c r="P18" s="79"/>
+      <c r="Q18" s="79"/>
+      <c r="R18" s="79"/>
+      <c r="S18" s="79"/>
       <c r="T18" s="30"/>
       <c r="U18" s="30"/>
       <c r="V18" s="30"/>
@@ -13643,16 +13643,16 @@
       <c r="I20" s="30"/>
       <c r="J20" s="30"/>
       <c r="K20" s="30"/>
-      <c r="L20" s="74" t="s">
+      <c r="L20" s="71" t="s">
         <v>1219</v>
       </c>
-      <c r="M20" s="74"/>
-      <c r="N20" s="74"/>
-      <c r="O20" s="74"/>
-      <c r="P20" s="74"/>
-      <c r="Q20" s="74"/>
-      <c r="R20" s="74"/>
-      <c r="S20" s="74"/>
+      <c r="M20" s="71"/>
+      <c r="N20" s="71"/>
+      <c r="O20" s="71"/>
+      <c r="P20" s="71"/>
+      <c r="Q20" s="71"/>
+      <c r="R20" s="71"/>
+      <c r="S20" s="71"/>
       <c r="T20" s="30"/>
       <c r="U20" s="30"/>
       <c r="V20" s="30"/>
@@ -13676,14 +13676,14 @@
       <c r="I21" s="30"/>
       <c r="J21" s="30"/>
       <c r="K21" s="30"/>
-      <c r="L21" s="74"/>
-      <c r="M21" s="74"/>
-      <c r="N21" s="74"/>
-      <c r="O21" s="74"/>
-      <c r="P21" s="74"/>
-      <c r="Q21" s="74"/>
-      <c r="R21" s="74"/>
-      <c r="S21" s="74"/>
+      <c r="L21" s="71"/>
+      <c r="M21" s="71"/>
+      <c r="N21" s="71"/>
+      <c r="O21" s="71"/>
+      <c r="P21" s="71"/>
+      <c r="Q21" s="71"/>
+      <c r="R21" s="71"/>
+      <c r="S21" s="71"/>
       <c r="T21" s="30"/>
       <c r="U21" s="30"/>
       <c r="V21" s="30"/>
@@ -13738,16 +13738,16 @@
       <c r="I23" s="30"/>
       <c r="J23" s="30"/>
       <c r="K23" s="30"/>
-      <c r="L23" s="72" t="s">
+      <c r="L23" s="80" t="s">
         <v>1220</v>
       </c>
-      <c r="M23" s="72"/>
-      <c r="N23" s="72"/>
-      <c r="O23" s="72"/>
-      <c r="P23" s="72"/>
-      <c r="Q23" s="72"/>
-      <c r="R23" s="72"/>
-      <c r="S23" s="72"/>
+      <c r="M23" s="80"/>
+      <c r="N23" s="80"/>
+      <c r="O23" s="80"/>
+      <c r="P23" s="80"/>
+      <c r="Q23" s="80"/>
+      <c r="R23" s="80"/>
+      <c r="S23" s="80"/>
       <c r="T23" s="30"/>
       <c r="U23" s="30"/>
       <c r="V23" s="30"/>
@@ -13771,14 +13771,14 @@
       <c r="I24" s="30"/>
       <c r="J24" s="30"/>
       <c r="K24" s="30"/>
-      <c r="L24" s="72"/>
-      <c r="M24" s="72"/>
-      <c r="N24" s="72"/>
-      <c r="O24" s="72"/>
-      <c r="P24" s="72"/>
-      <c r="Q24" s="72"/>
-      <c r="R24" s="72"/>
-      <c r="S24" s="72"/>
+      <c r="L24" s="80"/>
+      <c r="M24" s="80"/>
+      <c r="N24" s="80"/>
+      <c r="O24" s="80"/>
+      <c r="P24" s="80"/>
+      <c r="Q24" s="80"/>
+      <c r="R24" s="80"/>
+      <c r="S24" s="80"/>
       <c r="T24" s="30"/>
       <c r="U24" s="30"/>
       <c r="V24" s="30"/>
@@ -13948,40 +13948,40 @@
     </row>
     <row r="31" spans="1:29" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="30"/>
-      <c r="B31" s="73" t="s">
+      <c r="B31" s="77" t="s">
         <v>1221</v>
       </c>
-      <c r="C31" s="73"/>
-      <c r="D31" s="73"/>
-      <c r="E31" s="73"/>
-      <c r="F31" s="73"/>
-      <c r="G31" s="73"/>
-      <c r="H31" s="73"/>
-      <c r="I31" s="73"/>
+      <c r="C31" s="77"/>
+      <c r="D31" s="77"/>
+      <c r="E31" s="77"/>
+      <c r="F31" s="77"/>
+      <c r="G31" s="77"/>
+      <c r="H31" s="77"/>
+      <c r="I31" s="77"/>
       <c r="J31" s="30"/>
       <c r="K31" s="30"/>
-      <c r="L31" s="74" t="s">
+      <c r="L31" s="71" t="s">
         <v>1222</v>
       </c>
-      <c r="M31" s="74"/>
-      <c r="N31" s="74"/>
-      <c r="O31" s="74"/>
-      <c r="P31" s="74"/>
-      <c r="Q31" s="74"/>
-      <c r="R31" s="74"/>
-      <c r="S31" s="74"/>
+      <c r="M31" s="71"/>
+      <c r="N31" s="71"/>
+      <c r="O31" s="71"/>
+      <c r="P31" s="71"/>
+      <c r="Q31" s="71"/>
+      <c r="R31" s="71"/>
+      <c r="S31" s="71"/>
       <c r="T31" s="30"/>
       <c r="U31" s="30"/>
-      <c r="V31" s="74" t="s">
+      <c r="V31" s="71" t="s">
         <v>1223</v>
       </c>
-      <c r="W31" s="75"/>
-      <c r="X31" s="75"/>
-      <c r="Y31" s="75"/>
-      <c r="Z31" s="75"/>
-      <c r="AA31" s="75"/>
-      <c r="AB31" s="75"/>
-      <c r="AC31" s="75"/>
+      <c r="W31" s="79"/>
+      <c r="X31" s="79"/>
+      <c r="Y31" s="79"/>
+      <c r="Z31" s="79"/>
+      <c r="AA31" s="79"/>
+      <c r="AB31" s="79"/>
+      <c r="AC31" s="79"/>
     </row>
     <row r="32" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="30"/>
@@ -13995,68 +13995,68 @@
       <c r="I32" s="30"/>
       <c r="J32" s="30"/>
       <c r="K32" s="30"/>
-      <c r="L32" s="74"/>
-      <c r="M32" s="74"/>
-      <c r="N32" s="74"/>
-      <c r="O32" s="74"/>
-      <c r="P32" s="74"/>
-      <c r="Q32" s="74"/>
-      <c r="R32" s="74"/>
-      <c r="S32" s="74"/>
+      <c r="L32" s="71"/>
+      <c r="M32" s="71"/>
+      <c r="N32" s="71"/>
+      <c r="O32" s="71"/>
+      <c r="P32" s="71"/>
+      <c r="Q32" s="71"/>
+      <c r="R32" s="71"/>
+      <c r="S32" s="71"/>
       <c r="T32" s="30"/>
       <c r="U32" s="30"/>
-      <c r="V32" s="75"/>
-      <c r="W32" s="75"/>
-      <c r="X32" s="75"/>
-      <c r="Y32" s="75"/>
-      <c r="Z32" s="75"/>
-      <c r="AA32" s="75"/>
-      <c r="AB32" s="75"/>
-      <c r="AC32" s="75"/>
+      <c r="V32" s="79"/>
+      <c r="W32" s="79"/>
+      <c r="X32" s="79"/>
+      <c r="Y32" s="79"/>
+      <c r="Z32" s="79"/>
+      <c r="AA32" s="79"/>
+      <c r="AB32" s="79"/>
+      <c r="AC32" s="79"/>
     </row>
     <row r="33" spans="1:29" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="30"/>
-      <c r="B33" s="71" t="s">
+      <c r="B33" s="74" t="s">
         <v>1224</v>
       </c>
-      <c r="C33" s="71"/>
-      <c r="D33" s="71"/>
-      <c r="E33" s="71"/>
-      <c r="F33" s="71"/>
-      <c r="G33" s="71"/>
-      <c r="H33" s="71"/>
-      <c r="I33" s="71"/>
+      <c r="C33" s="74"/>
+      <c r="D33" s="74"/>
+      <c r="E33" s="74"/>
+      <c r="F33" s="74"/>
+      <c r="G33" s="74"/>
+      <c r="H33" s="74"/>
+      <c r="I33" s="74"/>
       <c r="J33" s="30"/>
       <c r="K33" s="30"/>
-      <c r="L33" s="74"/>
-      <c r="M33" s="74"/>
-      <c r="N33" s="74"/>
-      <c r="O33" s="74"/>
-      <c r="P33" s="74"/>
-      <c r="Q33" s="74"/>
-      <c r="R33" s="74"/>
-      <c r="S33" s="74"/>
+      <c r="L33" s="71"/>
+      <c r="M33" s="71"/>
+      <c r="N33" s="71"/>
+      <c r="O33" s="71"/>
+      <c r="P33" s="71"/>
+      <c r="Q33" s="71"/>
+      <c r="R33" s="71"/>
+      <c r="S33" s="71"/>
       <c r="T33" s="30"/>
       <c r="U33" s="30"/>
-      <c r="V33" s="75"/>
-      <c r="W33" s="75"/>
-      <c r="X33" s="75"/>
-      <c r="Y33" s="75"/>
-      <c r="Z33" s="75"/>
-      <c r="AA33" s="75"/>
-      <c r="AB33" s="75"/>
-      <c r="AC33" s="75"/>
+      <c r="V33" s="79"/>
+      <c r="W33" s="79"/>
+      <c r="X33" s="79"/>
+      <c r="Y33" s="79"/>
+      <c r="Z33" s="79"/>
+      <c r="AA33" s="79"/>
+      <c r="AB33" s="79"/>
+      <c r="AC33" s="79"/>
     </row>
     <row r="34" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="30"/>
-      <c r="B34" s="71"/>
-      <c r="C34" s="71"/>
-      <c r="D34" s="71"/>
-      <c r="E34" s="71"/>
-      <c r="F34" s="71"/>
-      <c r="G34" s="71"/>
-      <c r="H34" s="71"/>
-      <c r="I34" s="71"/>
+      <c r="B34" s="74"/>
+      <c r="C34" s="74"/>
+      <c r="D34" s="74"/>
+      <c r="E34" s="74"/>
+      <c r="F34" s="74"/>
+      <c r="G34" s="74"/>
+      <c r="H34" s="74"/>
+      <c r="I34" s="74"/>
       <c r="J34" s="30"/>
       <c r="K34" s="30"/>
       <c r="L34" s="30"/>
@@ -14090,28 +14090,28 @@
       <c r="I35" s="30"/>
       <c r="J35" s="30"/>
       <c r="K35" s="30"/>
-      <c r="L35" s="74" t="s">
+      <c r="L35" s="71" t="s">
         <v>1225</v>
       </c>
-      <c r="M35" s="74"/>
-      <c r="N35" s="74"/>
-      <c r="O35" s="74"/>
-      <c r="P35" s="74"/>
-      <c r="Q35" s="74"/>
-      <c r="R35" s="74"/>
-      <c r="S35" s="74"/>
+      <c r="M35" s="71"/>
+      <c r="N35" s="71"/>
+      <c r="O35" s="71"/>
+      <c r="P35" s="71"/>
+      <c r="Q35" s="71"/>
+      <c r="R35" s="71"/>
+      <c r="S35" s="71"/>
       <c r="T35" s="30"/>
       <c r="U35" s="30"/>
-      <c r="V35" s="71" t="s">
+      <c r="V35" s="74" t="s">
         <v>1226</v>
       </c>
-      <c r="W35" s="71"/>
-      <c r="X35" s="71"/>
-      <c r="Y35" s="71"/>
-      <c r="Z35" s="71"/>
-      <c r="AA35" s="71"/>
-      <c r="AB35" s="71"/>
-      <c r="AC35" s="71"/>
+      <c r="W35" s="74"/>
+      <c r="X35" s="74"/>
+      <c r="Y35" s="74"/>
+      <c r="Z35" s="74"/>
+      <c r="AA35" s="74"/>
+      <c r="AB35" s="74"/>
+      <c r="AC35" s="74"/>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A36" s="30"/>
@@ -14125,24 +14125,24 @@
       <c r="I36" s="30"/>
       <c r="J36" s="30"/>
       <c r="K36" s="30"/>
-      <c r="L36" s="74"/>
-      <c r="M36" s="74"/>
-      <c r="N36" s="74"/>
-      <c r="O36" s="74"/>
-      <c r="P36" s="74"/>
-      <c r="Q36" s="74"/>
-      <c r="R36" s="74"/>
-      <c r="S36" s="74"/>
+      <c r="L36" s="71"/>
+      <c r="M36" s="71"/>
+      <c r="N36" s="71"/>
+      <c r="O36" s="71"/>
+      <c r="P36" s="71"/>
+      <c r="Q36" s="71"/>
+      <c r="R36" s="71"/>
+      <c r="S36" s="71"/>
       <c r="T36" s="30"/>
       <c r="U36" s="30"/>
-      <c r="V36" s="71"/>
-      <c r="W36" s="71"/>
-      <c r="X36" s="71"/>
-      <c r="Y36" s="71"/>
-      <c r="Z36" s="71"/>
-      <c r="AA36" s="71"/>
-      <c r="AB36" s="71"/>
-      <c r="AC36" s="71"/>
+      <c r="V36" s="74"/>
+      <c r="W36" s="74"/>
+      <c r="X36" s="74"/>
+      <c r="Y36" s="74"/>
+      <c r="Z36" s="74"/>
+      <c r="AA36" s="74"/>
+      <c r="AB36" s="74"/>
+      <c r="AC36" s="74"/>
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A37" s="30"/>
@@ -14156,14 +14156,14 @@
       <c r="I37" s="30"/>
       <c r="J37" s="30"/>
       <c r="K37" s="30"/>
-      <c r="L37" s="74"/>
-      <c r="M37" s="74"/>
-      <c r="N37" s="74"/>
-      <c r="O37" s="74"/>
-      <c r="P37" s="74"/>
-      <c r="Q37" s="74"/>
-      <c r="R37" s="74"/>
-      <c r="S37" s="74"/>
+      <c r="L37" s="71"/>
+      <c r="M37" s="71"/>
+      <c r="N37" s="71"/>
+      <c r="O37" s="71"/>
+      <c r="P37" s="71"/>
+      <c r="Q37" s="71"/>
+      <c r="R37" s="71"/>
+      <c r="S37" s="71"/>
       <c r="T37" s="30"/>
       <c r="U37" s="30"/>
       <c r="V37" s="30"/>
@@ -14187,26 +14187,26 @@
       <c r="I38" s="30"/>
       <c r="J38" s="30"/>
       <c r="K38" s="30"/>
-      <c r="L38" s="74"/>
-      <c r="M38" s="74"/>
-      <c r="N38" s="74"/>
-      <c r="O38" s="74"/>
-      <c r="P38" s="74"/>
-      <c r="Q38" s="74"/>
-      <c r="R38" s="74"/>
-      <c r="S38" s="74"/>
+      <c r="L38" s="71"/>
+      <c r="M38" s="71"/>
+      <c r="N38" s="71"/>
+      <c r="O38" s="71"/>
+      <c r="P38" s="71"/>
+      <c r="Q38" s="71"/>
+      <c r="R38" s="71"/>
+      <c r="S38" s="71"/>
       <c r="T38" s="30"/>
       <c r="U38" s="30"/>
-      <c r="V38" s="72" t="s">
+      <c r="V38" s="80" t="s">
         <v>1219</v>
       </c>
-      <c r="W38" s="72"/>
-      <c r="X38" s="72"/>
-      <c r="Y38" s="72"/>
-      <c r="Z38" s="72"/>
-      <c r="AA38" s="72"/>
-      <c r="AB38" s="72"/>
-      <c r="AC38" s="72"/>
+      <c r="W38" s="80"/>
+      <c r="X38" s="80"/>
+      <c r="Y38" s="80"/>
+      <c r="Z38" s="80"/>
+      <c r="AA38" s="80"/>
+      <c r="AB38" s="80"/>
+      <c r="AC38" s="80"/>
     </row>
     <row r="39" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A39" s="30"/>
@@ -14220,26 +14220,26 @@
       <c r="I39" s="30"/>
       <c r="J39" s="30"/>
       <c r="K39" s="30"/>
-      <c r="L39" s="74" t="s">
+      <c r="L39" s="71" t="s">
         <v>1227</v>
       </c>
-      <c r="M39" s="74"/>
-      <c r="N39" s="74"/>
-      <c r="O39" s="74"/>
-      <c r="P39" s="74"/>
-      <c r="Q39" s="74"/>
-      <c r="R39" s="74"/>
-      <c r="S39" s="74"/>
+      <c r="M39" s="71"/>
+      <c r="N39" s="71"/>
+      <c r="O39" s="71"/>
+      <c r="P39" s="71"/>
+      <c r="Q39" s="71"/>
+      <c r="R39" s="71"/>
+      <c r="S39" s="71"/>
       <c r="T39" s="30"/>
       <c r="U39" s="30"/>
-      <c r="V39" s="72"/>
-      <c r="W39" s="72"/>
-      <c r="X39" s="72"/>
-      <c r="Y39" s="72"/>
-      <c r="Z39" s="72"/>
-      <c r="AA39" s="72"/>
-      <c r="AB39" s="72"/>
-      <c r="AC39" s="72"/>
+      <c r="V39" s="80"/>
+      <c r="W39" s="80"/>
+      <c r="X39" s="80"/>
+      <c r="Y39" s="80"/>
+      <c r="Z39" s="80"/>
+      <c r="AA39" s="80"/>
+      <c r="AB39" s="80"/>
+      <c r="AC39" s="80"/>
     </row>
     <row r="40" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A40" s="30"/>
@@ -14253,14 +14253,14 @@
       <c r="I40" s="30"/>
       <c r="J40" s="30"/>
       <c r="K40" s="30"/>
-      <c r="L40" s="74"/>
-      <c r="M40" s="74"/>
-      <c r="N40" s="74"/>
-      <c r="O40" s="74"/>
-      <c r="P40" s="74"/>
-      <c r="Q40" s="74"/>
-      <c r="R40" s="74"/>
-      <c r="S40" s="74"/>
+      <c r="L40" s="71"/>
+      <c r="M40" s="71"/>
+      <c r="N40" s="71"/>
+      <c r="O40" s="71"/>
+      <c r="P40" s="71"/>
+      <c r="Q40" s="71"/>
+      <c r="R40" s="71"/>
+      <c r="S40" s="71"/>
       <c r="T40" s="30"/>
       <c r="U40" s="30"/>
       <c r="V40" s="30"/>
@@ -14284,28 +14284,28 @@
       <c r="I41" s="30"/>
       <c r="J41" s="30"/>
       <c r="K41" s="30"/>
-      <c r="L41" s="74" t="s">
+      <c r="L41" s="71" t="s">
         <v>1228</v>
       </c>
-      <c r="M41" s="74"/>
-      <c r="N41" s="74"/>
-      <c r="O41" s="74"/>
-      <c r="P41" s="74"/>
-      <c r="Q41" s="74"/>
-      <c r="R41" s="74"/>
-      <c r="S41" s="74"/>
+      <c r="M41" s="71"/>
+      <c r="N41" s="71"/>
+      <c r="O41" s="71"/>
+      <c r="P41" s="71"/>
+      <c r="Q41" s="71"/>
+      <c r="R41" s="71"/>
+      <c r="S41" s="71"/>
       <c r="T41" s="30"/>
       <c r="U41" s="30"/>
-      <c r="V41" s="74" t="s">
+      <c r="V41" s="71" t="s">
         <v>1229</v>
       </c>
-      <c r="W41" s="74"/>
-      <c r="X41" s="74"/>
-      <c r="Y41" s="74"/>
-      <c r="Z41" s="74"/>
-      <c r="AA41" s="74"/>
-      <c r="AB41" s="74"/>
-      <c r="AC41" s="74"/>
+      <c r="W41" s="71"/>
+      <c r="X41" s="71"/>
+      <c r="Y41" s="71"/>
+      <c r="Z41" s="71"/>
+      <c r="AA41" s="71"/>
+      <c r="AB41" s="71"/>
+      <c r="AC41" s="71"/>
     </row>
     <row r="42" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="30"/>
@@ -14319,24 +14319,24 @@
       <c r="I42" s="30"/>
       <c r="J42" s="30"/>
       <c r="K42" s="30"/>
-      <c r="L42" s="74"/>
-      <c r="M42" s="74"/>
-      <c r="N42" s="74"/>
-      <c r="O42" s="74"/>
-      <c r="P42" s="74"/>
-      <c r="Q42" s="74"/>
-      <c r="R42" s="74"/>
-      <c r="S42" s="74"/>
+      <c r="L42" s="71"/>
+      <c r="M42" s="71"/>
+      <c r="N42" s="71"/>
+      <c r="O42" s="71"/>
+      <c r="P42" s="71"/>
+      <c r="Q42" s="71"/>
+      <c r="R42" s="71"/>
+      <c r="S42" s="71"/>
       <c r="T42" s="30"/>
       <c r="U42" s="30"/>
-      <c r="V42" s="74"/>
-      <c r="W42" s="74"/>
-      <c r="X42" s="74"/>
-      <c r="Y42" s="74"/>
-      <c r="Z42" s="74"/>
-      <c r="AA42" s="74"/>
-      <c r="AB42" s="74"/>
-      <c r="AC42" s="74"/>
+      <c r="V42" s="71"/>
+      <c r="W42" s="71"/>
+      <c r="X42" s="71"/>
+      <c r="Y42" s="71"/>
+      <c r="Z42" s="71"/>
+      <c r="AA42" s="71"/>
+      <c r="AB42" s="71"/>
+      <c r="AC42" s="71"/>
     </row>
     <row r="43" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="30"/>
@@ -14350,26 +14350,26 @@
       <c r="I43" s="30"/>
       <c r="J43" s="30"/>
       <c r="K43" s="30"/>
-      <c r="L43" s="72" t="s">
+      <c r="L43" s="80" t="s">
         <v>1230</v>
       </c>
-      <c r="M43" s="72"/>
-      <c r="N43" s="72"/>
-      <c r="O43" s="72"/>
-      <c r="P43" s="72"/>
-      <c r="Q43" s="72"/>
-      <c r="R43" s="72"/>
-      <c r="S43" s="72"/>
+      <c r="M43" s="80"/>
+      <c r="N43" s="80"/>
+      <c r="O43" s="80"/>
+      <c r="P43" s="80"/>
+      <c r="Q43" s="80"/>
+      <c r="R43" s="80"/>
+      <c r="S43" s="80"/>
       <c r="T43" s="30"/>
       <c r="U43" s="30"/>
-      <c r="V43" s="74"/>
-      <c r="W43" s="74"/>
-      <c r="X43" s="74"/>
-      <c r="Y43" s="74"/>
-      <c r="Z43" s="74"/>
-      <c r="AA43" s="74"/>
-      <c r="AB43" s="74"/>
-      <c r="AC43" s="74"/>
+      <c r="V43" s="71"/>
+      <c r="W43" s="71"/>
+      <c r="X43" s="71"/>
+      <c r="Y43" s="71"/>
+      <c r="Z43" s="71"/>
+      <c r="AA43" s="71"/>
+      <c r="AB43" s="71"/>
+      <c r="AC43" s="71"/>
     </row>
     <row r="44" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="30"/>
@@ -14383,26 +14383,26 @@
       <c r="I44" s="30"/>
       <c r="J44" s="30"/>
       <c r="K44" s="30"/>
-      <c r="L44" s="72"/>
-      <c r="M44" s="72"/>
-      <c r="N44" s="72"/>
-      <c r="O44" s="72"/>
-      <c r="P44" s="72"/>
-      <c r="Q44" s="72"/>
-      <c r="R44" s="72"/>
-      <c r="S44" s="72"/>
+      <c r="L44" s="80"/>
+      <c r="M44" s="80"/>
+      <c r="N44" s="80"/>
+      <c r="O44" s="80"/>
+      <c r="P44" s="80"/>
+      <c r="Q44" s="80"/>
+      <c r="R44" s="80"/>
+      <c r="S44" s="80"/>
       <c r="T44" s="30"/>
       <c r="U44" s="30"/>
-      <c r="V44" s="71" t="s">
+      <c r="V44" s="74" t="s">
         <v>1231</v>
       </c>
-      <c r="W44" s="71"/>
-      <c r="X44" s="71"/>
-      <c r="Y44" s="71"/>
-      <c r="Z44" s="71"/>
-      <c r="AA44" s="71"/>
-      <c r="AB44" s="71"/>
-      <c r="AC44" s="71"/>
+      <c r="W44" s="74"/>
+      <c r="X44" s="74"/>
+      <c r="Y44" s="74"/>
+      <c r="Z44" s="74"/>
+      <c r="AA44" s="74"/>
+      <c r="AB44" s="74"/>
+      <c r="AC44" s="74"/>
     </row>
     <row r="45" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A45" s="30"/>
@@ -14416,24 +14416,24 @@
       <c r="I45" s="30"/>
       <c r="J45" s="30"/>
       <c r="K45" s="30"/>
-      <c r="L45" s="72"/>
-      <c r="M45" s="72"/>
-      <c r="N45" s="72"/>
-      <c r="O45" s="72"/>
-      <c r="P45" s="72"/>
-      <c r="Q45" s="72"/>
-      <c r="R45" s="72"/>
-      <c r="S45" s="72"/>
+      <c r="L45" s="80"/>
+      <c r="M45" s="80"/>
+      <c r="N45" s="80"/>
+      <c r="O45" s="80"/>
+      <c r="P45" s="80"/>
+      <c r="Q45" s="80"/>
+      <c r="R45" s="80"/>
+      <c r="S45" s="80"/>
       <c r="T45" s="30"/>
       <c r="U45" s="30"/>
-      <c r="V45" s="71"/>
-      <c r="W45" s="71"/>
-      <c r="X45" s="71"/>
-      <c r="Y45" s="71"/>
-      <c r="Z45" s="71"/>
-      <c r="AA45" s="71"/>
-      <c r="AB45" s="71"/>
-      <c r="AC45" s="71"/>
+      <c r="V45" s="74"/>
+      <c r="W45" s="74"/>
+      <c r="X45" s="74"/>
+      <c r="Y45" s="74"/>
+      <c r="Z45" s="74"/>
+      <c r="AA45" s="74"/>
+      <c r="AB45" s="74"/>
+      <c r="AC45" s="74"/>
     </row>
     <row r="46" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="30"/>
@@ -14447,16 +14447,16 @@
       <c r="I46" s="30"/>
       <c r="J46" s="30"/>
       <c r="K46" s="30"/>
-      <c r="L46" s="74" t="s">
+      <c r="L46" s="71" t="s">
         <v>1232</v>
       </c>
-      <c r="M46" s="74"/>
-      <c r="N46" s="74"/>
-      <c r="O46" s="74"/>
-      <c r="P46" s="74"/>
-      <c r="Q46" s="74"/>
-      <c r="R46" s="74"/>
-      <c r="S46" s="74"/>
+      <c r="M46" s="71"/>
+      <c r="N46" s="71"/>
+      <c r="O46" s="71"/>
+      <c r="P46" s="71"/>
+      <c r="Q46" s="71"/>
+      <c r="R46" s="71"/>
+      <c r="S46" s="71"/>
       <c r="T46" s="30"/>
       <c r="U46" s="30"/>
       <c r="V46" s="30"/>
@@ -14470,26 +14470,26 @@
     </row>
     <row r="47" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="30"/>
-      <c r="B47" s="71" t="s">
+      <c r="B47" s="74" t="s">
         <v>1233</v>
       </c>
-      <c r="C47" s="71"/>
-      <c r="D47" s="71"/>
-      <c r="E47" s="71"/>
-      <c r="F47" s="71"/>
-      <c r="G47" s="71"/>
-      <c r="H47" s="71"/>
-      <c r="I47" s="71"/>
+      <c r="C47" s="74"/>
+      <c r="D47" s="74"/>
+      <c r="E47" s="74"/>
+      <c r="F47" s="74"/>
+      <c r="G47" s="74"/>
+      <c r="H47" s="74"/>
+      <c r="I47" s="74"/>
       <c r="J47" s="30"/>
       <c r="K47" s="30"/>
-      <c r="L47" s="74"/>
-      <c r="M47" s="74"/>
-      <c r="N47" s="74"/>
-      <c r="O47" s="74"/>
-      <c r="P47" s="74"/>
-      <c r="Q47" s="74"/>
-      <c r="R47" s="74"/>
-      <c r="S47" s="74"/>
+      <c r="L47" s="71"/>
+      <c r="M47" s="71"/>
+      <c r="N47" s="71"/>
+      <c r="O47" s="71"/>
+      <c r="P47" s="71"/>
+      <c r="Q47" s="71"/>
+      <c r="R47" s="71"/>
+      <c r="S47" s="71"/>
       <c r="T47" s="30"/>
       <c r="U47" s="30"/>
       <c r="V47" s="30"/>
@@ -14503,24 +14503,24 @@
     </row>
     <row r="48" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="30"/>
-      <c r="B48" s="71"/>
-      <c r="C48" s="71"/>
-      <c r="D48" s="71"/>
-      <c r="E48" s="71"/>
-      <c r="F48" s="71"/>
-      <c r="G48" s="71"/>
-      <c r="H48" s="71"/>
-      <c r="I48" s="71"/>
+      <c r="B48" s="74"/>
+      <c r="C48" s="74"/>
+      <c r="D48" s="74"/>
+      <c r="E48" s="74"/>
+      <c r="F48" s="74"/>
+      <c r="G48" s="74"/>
+      <c r="H48" s="74"/>
+      <c r="I48" s="74"/>
       <c r="J48" s="30"/>
       <c r="K48" s="30"/>
-      <c r="L48" s="74"/>
-      <c r="M48" s="74"/>
-      <c r="N48" s="74"/>
-      <c r="O48" s="74"/>
-      <c r="P48" s="74"/>
-      <c r="Q48" s="74"/>
-      <c r="R48" s="74"/>
-      <c r="S48" s="74"/>
+      <c r="L48" s="71"/>
+      <c r="M48" s="71"/>
+      <c r="N48" s="71"/>
+      <c r="O48" s="71"/>
+      <c r="P48" s="71"/>
+      <c r="Q48" s="71"/>
+      <c r="R48" s="71"/>
+      <c r="S48" s="71"/>
       <c r="T48" s="30"/>
       <c r="U48" s="30"/>
       <c r="V48" s="30"/>
@@ -14534,14 +14534,14 @@
     </row>
     <row r="49" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="30"/>
-      <c r="B49" s="71"/>
-      <c r="C49" s="71"/>
-      <c r="D49" s="71"/>
-      <c r="E49" s="71"/>
-      <c r="F49" s="71"/>
-      <c r="G49" s="71"/>
-      <c r="H49" s="71"/>
-      <c r="I49" s="71"/>
+      <c r="B49" s="74"/>
+      <c r="C49" s="74"/>
+      <c r="D49" s="74"/>
+      <c r="E49" s="74"/>
+      <c r="F49" s="74"/>
+      <c r="G49" s="74"/>
+      <c r="H49" s="74"/>
+      <c r="I49" s="74"/>
       <c r="J49" s="30"/>
       <c r="K49" s="30"/>
       <c r="L49" s="30"/>
@@ -14565,14 +14565,14 @@
     </row>
     <row r="50" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A50" s="30"/>
-      <c r="B50" s="71"/>
-      <c r="C50" s="71"/>
-      <c r="D50" s="71"/>
-      <c r="E50" s="71"/>
-      <c r="F50" s="71"/>
-      <c r="G50" s="71"/>
-      <c r="H50" s="71"/>
-      <c r="I50" s="71"/>
+      <c r="B50" s="74"/>
+      <c r="C50" s="74"/>
+      <c r="D50" s="74"/>
+      <c r="E50" s="74"/>
+      <c r="F50" s="74"/>
+      <c r="G50" s="74"/>
+      <c r="H50" s="74"/>
+      <c r="I50" s="74"/>
       <c r="J50" s="30"/>
       <c r="K50" s="30"/>
       <c r="L50" s="30"/>
@@ -14596,14 +14596,14 @@
     </row>
     <row r="51" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A51" s="30"/>
-      <c r="B51" s="71"/>
-      <c r="C51" s="71"/>
-      <c r="D51" s="71"/>
-      <c r="E51" s="71"/>
-      <c r="F51" s="71"/>
-      <c r="G51" s="71"/>
-      <c r="H51" s="71"/>
-      <c r="I51" s="71"/>
+      <c r="B51" s="74"/>
+      <c r="C51" s="74"/>
+      <c r="D51" s="74"/>
+      <c r="E51" s="74"/>
+      <c r="F51" s="74"/>
+      <c r="G51" s="74"/>
+      <c r="H51" s="74"/>
+      <c r="I51" s="74"/>
       <c r="J51" s="30"/>
       <c r="K51" s="30"/>
       <c r="L51" s="30"/>
@@ -15758,18 +15758,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="Ni3oRhRFSHLqcHPeDMM9oJPhO6WfMxTCuA0QUr0aYxZ5GIVg5SnJ0DmCKugqbXaRKsIRpp0xaviZSFtXtsEQYA==" saltValue="uU6zNIz4+Gs4uisLnne5sQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="27">
-    <mergeCell ref="L20:S21"/>
-    <mergeCell ref="B4:I4"/>
-    <mergeCell ref="V4:AC4"/>
-    <mergeCell ref="B5:I5"/>
-    <mergeCell ref="V5:AC5"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="V7:AC7"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="V8:AC8"/>
-    <mergeCell ref="V10:AC10"/>
-    <mergeCell ref="L16:S17"/>
-    <mergeCell ref="L18:S18"/>
     <mergeCell ref="B47:I51"/>
     <mergeCell ref="L23:S24"/>
     <mergeCell ref="B31:I31"/>
@@ -15785,6 +15773,18 @@
     <mergeCell ref="L43:S45"/>
     <mergeCell ref="V44:AC45"/>
     <mergeCell ref="L46:S48"/>
+    <mergeCell ref="L20:S21"/>
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="V4:AC4"/>
+    <mergeCell ref="B5:I5"/>
+    <mergeCell ref="V5:AC5"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="V7:AC7"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="V8:AC8"/>
+    <mergeCell ref="V10:AC10"/>
+    <mergeCell ref="L16:S17"/>
+    <mergeCell ref="L18:S18"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1" xr:uid="{5E7C7A05-D050-4790-AD5A-2C904F987D3F}"/>
@@ -16061,7 +16061,7 @@
   <dimension ref="A1:AD63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
changed test data to only contain valid user types
</commit_message>
<xml_diff>
--- a/src/integrationTest/resources/Staff Data Upload With All Valid Rows.xlsx
+++ b/src/integrationTest/resources/Staff Data Upload With All Valid Rows.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_900458/Documents/HMCTS/rd-caseworker-ref-api/src/integrationTest/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukaszwolski/rd-repos/rd-caseworker-ref-api/src/integrationTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FA2F63-12C5-DC4D-BE48-ACBD6AEAE010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F18FFCA-18BB-E147-AD35-03762F092B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" activeTab="3" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
+    <workbookView xWindow="200" yWindow="-26260" windowWidth="38380" windowHeight="22360" activeTab="3" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
   </bookViews>
   <sheets>
     <sheet name="VERSION" sheetId="13" r:id="rId1"/>
@@ -42,8 +42,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -3609,9 +3613,6 @@
   </si>
   <si>
     <t>Secondary Location ID</t>
-  </si>
-  <si>
-    <t>CTRT</t>
   </si>
   <si>
     <t>Month</t>
@@ -3965,6 +3966,9 @@
   </si>
   <si>
     <t>Senior Legal Caseworker</t>
+  </si>
+  <si>
+    <t>Future Operations</t>
   </si>
 </sst>
 </file>
@@ -4395,7 +4399,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -4464,7 +4468,7 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4483,7 +4487,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -4501,18 +4505,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
@@ -4528,10 +4528,10 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4589,19 +4589,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -4609,12 +4597,24 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -12653,7 +12653,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="VERSION"/>
@@ -12684,9 +12684,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -12724,7 +12724,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -12830,7 +12830,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -12972,7 +12972,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -12999,64 +12999,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="39" t="s">
+        <v>1188</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="41"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="42"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="45" t="s">
+        <v>1185</v>
+      </c>
+      <c r="B3" s="50" t="s">
+        <v>1191</v>
+      </c>
+      <c r="C3" s="43"/>
+      <c r="D3" s="44"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="45" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B4" s="50">
+        <v>2021</v>
+      </c>
+      <c r="C4" s="43"/>
+      <c r="D4" s="44"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="45" t="s">
+        <v>1187</v>
+      </c>
+      <c r="B5" s="46" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C5" s="43"/>
+      <c r="D5" s="44"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="45" t="s">
         <v>1189</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="43"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="44"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="46"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="47" t="s">
-        <v>1186</v>
-      </c>
-      <c r="B3" s="52" t="s">
-        <v>1192</v>
-      </c>
-      <c r="C3" s="45"/>
-      <c r="D3" s="46"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="47" t="s">
-        <v>1187</v>
-      </c>
-      <c r="B4" s="52">
-        <v>2021</v>
-      </c>
-      <c r="C4" s="45"/>
-      <c r="D4" s="46"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="47" t="s">
-        <v>1188</v>
-      </c>
-      <c r="B5" s="48" t="s">
-        <v>1191</v>
-      </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="46"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="47" t="s">
-        <v>1190</v>
-      </c>
-      <c r="B6" s="52" t="s">
-        <v>1224</v>
-      </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="46"/>
+      <c r="B6" s="50" t="s">
+        <v>1223</v>
+      </c>
+      <c r="C6" s="43"/>
+      <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="49"/>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="51"/>
+      <c r="A7" s="47"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="49"/>
     </row>
     <row r="8" spans="1:4" s="31" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="9" spans="1:4" s="31" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -13240,60 +13240,60 @@
       <c r="AB3" s="29"/>
       <c r="AC3" s="29"/>
     </row>
-    <row r="4" spans="1:34" s="69" customFormat="1" ht="34.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="67"/>
-      <c r="B4" s="82" t="s">
+    <row r="4" spans="1:34" s="67" customFormat="1" ht="34.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="65"/>
+      <c r="B4" s="76" t="s">
+        <v>1197</v>
+      </c>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="64" t="s">
         <v>1198</v>
       </c>
-      <c r="C4" s="82"/>
-      <c r="D4" s="82"/>
-      <c r="E4" s="82"/>
-      <c r="F4" s="82"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="82"/>
-      <c r="J4" s="67"/>
-      <c r="K4" s="67"/>
-      <c r="L4" s="66" t="s">
+      <c r="M4" s="65"/>
+      <c r="N4" s="65"/>
+      <c r="O4" s="65"/>
+      <c r="P4" s="65"/>
+      <c r="Q4" s="65"/>
+      <c r="R4" s="65"/>
+      <c r="S4" s="65"/>
+      <c r="T4" s="65"/>
+      <c r="U4" s="65"/>
+      <c r="V4" s="76" t="s">
         <v>1199</v>
       </c>
-      <c r="M4" s="67"/>
-      <c r="N4" s="67"/>
-      <c r="O4" s="67"/>
-      <c r="P4" s="67"/>
-      <c r="Q4" s="67"/>
-      <c r="R4" s="67"/>
-      <c r="S4" s="67"/>
-      <c r="T4" s="67"/>
-      <c r="U4" s="67"/>
-      <c r="V4" s="82" t="s">
-        <v>1200</v>
-      </c>
-      <c r="W4" s="82"/>
-      <c r="X4" s="82"/>
-      <c r="Y4" s="82"/>
-      <c r="Z4" s="82"/>
-      <c r="AA4" s="82"/>
-      <c r="AB4" s="82"/>
-      <c r="AC4" s="82"/>
-      <c r="AD4" s="68"/>
-      <c r="AE4" s="68"/>
-      <c r="AF4" s="68"/>
-      <c r="AG4" s="68"/>
-      <c r="AH4" s="68"/>
+      <c r="W4" s="76"/>
+      <c r="X4" s="76"/>
+      <c r="Y4" s="76"/>
+      <c r="Z4" s="76"/>
+      <c r="AA4" s="76"/>
+      <c r="AB4" s="76"/>
+      <c r="AC4" s="76"/>
+      <c r="AD4" s="66"/>
+      <c r="AE4" s="66"/>
+      <c r="AF4" s="66"/>
+      <c r="AG4" s="66"/>
+      <c r="AH4" s="66"/>
     </row>
     <row r="5" spans="1:34" ht="31.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="29"/>
-      <c r="B5" s="83" t="s">
-        <v>1225</v>
-      </c>
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="77"/>
+      <c r="B5" s="77" t="s">
+        <v>1224</v>
+      </c>
+      <c r="C5" s="78"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="78"/>
+      <c r="I5" s="78"/>
       <c r="J5" s="29"/>
       <c r="K5" s="29"/>
       <c r="L5" s="29"/>
@@ -13306,16 +13306,16 @@
       <c r="S5" s="29"/>
       <c r="T5" s="29"/>
       <c r="U5" s="29"/>
-      <c r="V5" s="84" t="s">
-        <v>1201</v>
-      </c>
-      <c r="W5" s="77"/>
-      <c r="X5" s="77"/>
-      <c r="Y5" s="77"/>
-      <c r="Z5" s="77"/>
-      <c r="AA5" s="77"/>
-      <c r="AB5" s="77"/>
-      <c r="AC5" s="77"/>
+      <c r="V5" s="79" t="s">
+        <v>1200</v>
+      </c>
+      <c r="W5" s="78"/>
+      <c r="X5" s="78"/>
+      <c r="Y5" s="78"/>
+      <c r="Z5" s="78"/>
+      <c r="AA5" s="78"/>
+      <c r="AB5" s="78"/>
+      <c r="AC5" s="78"/>
     </row>
     <row r="6" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="29"/>
@@ -13339,27 +13339,27 @@
       <c r="S6" s="29"/>
       <c r="T6" s="29"/>
       <c r="U6" s="29"/>
-      <c r="V6" s="65"/>
-      <c r="W6" s="65"/>
-      <c r="X6" s="65"/>
-      <c r="Y6" s="65"/>
-      <c r="Z6" s="65"/>
-      <c r="AA6" s="65"/>
-      <c r="AB6" s="65"/>
-      <c r="AC6" s="65"/>
+      <c r="V6" s="63"/>
+      <c r="W6" s="63"/>
+      <c r="X6" s="63"/>
+      <c r="Y6" s="63"/>
+      <c r="Z6" s="63"/>
+      <c r="AA6" s="63"/>
+      <c r="AB6" s="63"/>
+      <c r="AC6" s="63"/>
     </row>
     <row r="7" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="29"/>
-      <c r="B7" s="85" t="s">
-        <v>1202</v>
-      </c>
-      <c r="C7" s="85"/>
-      <c r="D7" s="85"/>
-      <c r="E7" s="85"/>
-      <c r="F7" s="85"/>
-      <c r="G7" s="85"/>
-      <c r="H7" s="85"/>
-      <c r="I7" s="85"/>
+      <c r="B7" s="80" t="s">
+        <v>1201</v>
+      </c>
+      <c r="C7" s="80"/>
+      <c r="D7" s="80"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="80"/>
+      <c r="G7" s="80"/>
+      <c r="H7" s="80"/>
+      <c r="I7" s="80"/>
       <c r="J7" s="29"/>
       <c r="K7" s="29"/>
       <c r="L7" s="29"/>
@@ -13372,29 +13372,29 @@
       <c r="S7" s="29"/>
       <c r="T7" s="29"/>
       <c r="U7" s="29"/>
-      <c r="V7" s="85" t="s">
-        <v>1203</v>
-      </c>
-      <c r="W7" s="85"/>
-      <c r="X7" s="85"/>
-      <c r="Y7" s="85"/>
-      <c r="Z7" s="85"/>
-      <c r="AA7" s="85"/>
-      <c r="AB7" s="85"/>
-      <c r="AC7" s="85"/>
+      <c r="V7" s="80" t="s">
+        <v>1202</v>
+      </c>
+      <c r="W7" s="80"/>
+      <c r="X7" s="80"/>
+      <c r="Y7" s="80"/>
+      <c r="Z7" s="80"/>
+      <c r="AA7" s="80"/>
+      <c r="AB7" s="80"/>
+      <c r="AC7" s="80"/>
     </row>
     <row r="8" spans="1:34" ht="32.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="29"/>
-      <c r="B8" s="79" t="s">
-        <v>1204</v>
-      </c>
-      <c r="C8" s="79"/>
-      <c r="D8" s="79"/>
-      <c r="E8" s="79"/>
-      <c r="F8" s="79"/>
-      <c r="G8" s="79"/>
-      <c r="H8" s="79"/>
-      <c r="I8" s="79"/>
+      <c r="B8" s="81" t="s">
+        <v>1203</v>
+      </c>
+      <c r="C8" s="81"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="81"/>
+      <c r="G8" s="81"/>
+      <c r="H8" s="81"/>
+      <c r="I8" s="81"/>
       <c r="J8" s="29"/>
       <c r="K8" s="29"/>
       <c r="L8" s="29"/>
@@ -13407,16 +13407,16 @@
       <c r="S8" s="29"/>
       <c r="T8" s="29"/>
       <c r="U8" s="29"/>
-      <c r="V8" s="79" t="s">
-        <v>1205</v>
-      </c>
-      <c r="W8" s="79"/>
-      <c r="X8" s="79"/>
-      <c r="Y8" s="79"/>
-      <c r="Z8" s="79"/>
-      <c r="AA8" s="79"/>
-      <c r="AB8" s="79"/>
-      <c r="AC8" s="79"/>
+      <c r="V8" s="81" t="s">
+        <v>1204</v>
+      </c>
+      <c r="W8" s="81"/>
+      <c r="X8" s="81"/>
+      <c r="Y8" s="81"/>
+      <c r="Z8" s="81"/>
+      <c r="AA8" s="81"/>
+      <c r="AB8" s="81"/>
+      <c r="AC8" s="81"/>
     </row>
     <row r="9" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="29"/>
@@ -13440,14 +13440,14 @@
       <c r="S9" s="29"/>
       <c r="T9" s="29"/>
       <c r="U9" s="29"/>
-      <c r="V9" s="65"/>
-      <c r="W9" s="65"/>
-      <c r="X9" s="65"/>
-      <c r="Y9" s="65"/>
-      <c r="Z9" s="65"/>
-      <c r="AA9" s="65"/>
-      <c r="AB9" s="65"/>
-      <c r="AC9" s="65"/>
+      <c r="V9" s="63"/>
+      <c r="W9" s="63"/>
+      <c r="X9" s="63"/>
+      <c r="Y9" s="63"/>
+      <c r="Z9" s="63"/>
+      <c r="AA9" s="63"/>
+      <c r="AB9" s="63"/>
+      <c r="AC9" s="63"/>
     </row>
     <row r="10" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="29"/>
@@ -13471,16 +13471,16 @@
       <c r="S10" s="29"/>
       <c r="T10" s="29"/>
       <c r="U10" s="29"/>
-      <c r="V10" s="79" t="s">
-        <v>1206</v>
-      </c>
-      <c r="W10" s="79"/>
-      <c r="X10" s="79"/>
-      <c r="Y10" s="79"/>
-      <c r="Z10" s="79"/>
-      <c r="AA10" s="79"/>
-      <c r="AB10" s="79"/>
-      <c r="AC10" s="79"/>
+      <c r="V10" s="81" t="s">
+        <v>1205</v>
+      </c>
+      <c r="W10" s="81"/>
+      <c r="X10" s="81"/>
+      <c r="Y10" s="81"/>
+      <c r="Z10" s="81"/>
+      <c r="AA10" s="81"/>
+      <c r="AB10" s="81"/>
+      <c r="AC10" s="81"/>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A11" s="29"/>
@@ -13649,16 +13649,16 @@
       <c r="I16" s="29"/>
       <c r="J16" s="29"/>
       <c r="K16" s="29"/>
-      <c r="L16" s="80" t="s">
-        <v>1207</v>
-      </c>
-      <c r="M16" s="80"/>
-      <c r="N16" s="80"/>
-      <c r="O16" s="80"/>
-      <c r="P16" s="80"/>
-      <c r="Q16" s="80"/>
-      <c r="R16" s="80"/>
-      <c r="S16" s="80"/>
+      <c r="L16" s="75" t="s">
+        <v>1206</v>
+      </c>
+      <c r="M16" s="75"/>
+      <c r="N16" s="75"/>
+      <c r="O16" s="75"/>
+      <c r="P16" s="75"/>
+      <c r="Q16" s="75"/>
+      <c r="R16" s="75"/>
+      <c r="S16" s="75"/>
       <c r="T16" s="29"/>
       <c r="U16" s="29"/>
       <c r="V16" s="29"/>
@@ -13682,14 +13682,14 @@
       <c r="I17" s="29"/>
       <c r="J17" s="29"/>
       <c r="K17" s="29"/>
-      <c r="L17" s="80"/>
-      <c r="M17" s="80"/>
-      <c r="N17" s="80"/>
-      <c r="O17" s="80"/>
-      <c r="P17" s="80"/>
-      <c r="Q17" s="80"/>
-      <c r="R17" s="80"/>
-      <c r="S17" s="80"/>
+      <c r="L17" s="75"/>
+      <c r="M17" s="75"/>
+      <c r="N17" s="75"/>
+      <c r="O17" s="75"/>
+      <c r="P17" s="75"/>
+      <c r="Q17" s="75"/>
+      <c r="R17" s="75"/>
+      <c r="S17" s="75"/>
       <c r="T17" s="29"/>
       <c r="U17" s="29"/>
       <c r="V17" s="29"/>
@@ -13713,16 +13713,16 @@
       <c r="I18" s="29"/>
       <c r="J18" s="29"/>
       <c r="K18" s="29"/>
-      <c r="L18" s="86" t="s">
-        <v>1208</v>
-      </c>
-      <c r="M18" s="81"/>
-      <c r="N18" s="81"/>
-      <c r="O18" s="81"/>
-      <c r="P18" s="81"/>
-      <c r="Q18" s="81"/>
-      <c r="R18" s="81"/>
-      <c r="S18" s="81"/>
+      <c r="L18" s="82" t="s">
+        <v>1207</v>
+      </c>
+      <c r="M18" s="83"/>
+      <c r="N18" s="83"/>
+      <c r="O18" s="83"/>
+      <c r="P18" s="83"/>
+      <c r="Q18" s="83"/>
+      <c r="R18" s="83"/>
+      <c r="S18" s="83"/>
       <c r="T18" s="29"/>
       <c r="U18" s="29"/>
       <c r="V18" s="29"/>
@@ -13746,14 +13746,14 @@
       <c r="I19" s="29"/>
       <c r="J19" s="29"/>
       <c r="K19" s="29"/>
-      <c r="L19" s="66"/>
-      <c r="M19" s="66"/>
-      <c r="N19" s="66"/>
-      <c r="O19" s="66"/>
-      <c r="P19" s="66"/>
-      <c r="Q19" s="66"/>
-      <c r="R19" s="66"/>
-      <c r="S19" s="66"/>
+      <c r="L19" s="64"/>
+      <c r="M19" s="64"/>
+      <c r="N19" s="64"/>
+      <c r="O19" s="64"/>
+      <c r="P19" s="64"/>
+      <c r="Q19" s="64"/>
+      <c r="R19" s="64"/>
+      <c r="S19" s="64"/>
       <c r="T19" s="29"/>
       <c r="U19" s="29"/>
       <c r="V19" s="29"/>
@@ -13777,16 +13777,16 @@
       <c r="I20" s="29"/>
       <c r="J20" s="29"/>
       <c r="K20" s="29"/>
-      <c r="L20" s="80" t="s">
-        <v>1209</v>
-      </c>
-      <c r="M20" s="80"/>
-      <c r="N20" s="80"/>
-      <c r="O20" s="80"/>
-      <c r="P20" s="80"/>
-      <c r="Q20" s="80"/>
-      <c r="R20" s="80"/>
-      <c r="S20" s="80"/>
+      <c r="L20" s="75" t="s">
+        <v>1208</v>
+      </c>
+      <c r="M20" s="75"/>
+      <c r="N20" s="75"/>
+      <c r="O20" s="75"/>
+      <c r="P20" s="75"/>
+      <c r="Q20" s="75"/>
+      <c r="R20" s="75"/>
+      <c r="S20" s="75"/>
       <c r="T20" s="29"/>
       <c r="U20" s="29"/>
       <c r="V20" s="29"/>
@@ -13810,14 +13810,14 @@
       <c r="I21" s="29"/>
       <c r="J21" s="29"/>
       <c r="K21" s="29"/>
-      <c r="L21" s="80"/>
-      <c r="M21" s="80"/>
-      <c r="N21" s="80"/>
-      <c r="O21" s="80"/>
-      <c r="P21" s="80"/>
-      <c r="Q21" s="80"/>
-      <c r="R21" s="80"/>
-      <c r="S21" s="80"/>
+      <c r="L21" s="75"/>
+      <c r="M21" s="75"/>
+      <c r="N21" s="75"/>
+      <c r="O21" s="75"/>
+      <c r="P21" s="75"/>
+      <c r="Q21" s="75"/>
+      <c r="R21" s="75"/>
+      <c r="S21" s="75"/>
       <c r="T21" s="29"/>
       <c r="U21" s="29"/>
       <c r="V21" s="29"/>
@@ -13841,14 +13841,14 @@
       <c r="I22" s="29"/>
       <c r="J22" s="29"/>
       <c r="K22" s="29"/>
-      <c r="L22" s="65"/>
-      <c r="M22" s="65"/>
-      <c r="N22" s="65"/>
-      <c r="O22" s="65"/>
-      <c r="P22" s="65"/>
-      <c r="Q22" s="65"/>
-      <c r="R22" s="65"/>
-      <c r="S22" s="65"/>
+      <c r="L22" s="63"/>
+      <c r="M22" s="63"/>
+      <c r="N22" s="63"/>
+      <c r="O22" s="63"/>
+      <c r="P22" s="63"/>
+      <c r="Q22" s="63"/>
+      <c r="R22" s="63"/>
+      <c r="S22" s="63"/>
       <c r="T22" s="29"/>
       <c r="U22" s="29"/>
       <c r="V22" s="29"/>
@@ -13872,16 +13872,16 @@
       <c r="I23" s="29"/>
       <c r="J23" s="29"/>
       <c r="K23" s="29"/>
-      <c r="L23" s="78" t="s">
-        <v>1210</v>
-      </c>
-      <c r="M23" s="78"/>
-      <c r="N23" s="78"/>
-      <c r="O23" s="78"/>
-      <c r="P23" s="78"/>
-      <c r="Q23" s="78"/>
-      <c r="R23" s="78"/>
-      <c r="S23" s="78"/>
+      <c r="L23" s="84" t="s">
+        <v>1209</v>
+      </c>
+      <c r="M23" s="84"/>
+      <c r="N23" s="84"/>
+      <c r="O23" s="84"/>
+      <c r="P23" s="84"/>
+      <c r="Q23" s="84"/>
+      <c r="R23" s="84"/>
+      <c r="S23" s="84"/>
       <c r="T23" s="29"/>
       <c r="U23" s="29"/>
       <c r="V23" s="29"/>
@@ -13905,14 +13905,14 @@
       <c r="I24" s="29"/>
       <c r="J24" s="29"/>
       <c r="K24" s="29"/>
-      <c r="L24" s="78"/>
-      <c r="M24" s="78"/>
-      <c r="N24" s="78"/>
-      <c r="O24" s="78"/>
-      <c r="P24" s="78"/>
-      <c r="Q24" s="78"/>
-      <c r="R24" s="78"/>
-      <c r="S24" s="78"/>
+      <c r="L24" s="84"/>
+      <c r="M24" s="84"/>
+      <c r="N24" s="84"/>
+      <c r="O24" s="84"/>
+      <c r="P24" s="84"/>
+      <c r="Q24" s="84"/>
+      <c r="R24" s="84"/>
+      <c r="S24" s="84"/>
       <c r="T24" s="29"/>
       <c r="U24" s="29"/>
       <c r="V24" s="29"/>
@@ -14082,40 +14082,40 @@
     </row>
     <row r="31" spans="1:29" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="29"/>
-      <c r="B31" s="79" t="s">
-        <v>1211</v>
-      </c>
-      <c r="C31" s="79"/>
-      <c r="D31" s="79"/>
-      <c r="E31" s="79"/>
-      <c r="F31" s="79"/>
-      <c r="G31" s="79"/>
-      <c r="H31" s="79"/>
-      <c r="I31" s="79"/>
+      <c r="B31" s="81" t="s">
+        <v>1210</v>
+      </c>
+      <c r="C31" s="81"/>
+      <c r="D31" s="81"/>
+      <c r="E31" s="81"/>
+      <c r="F31" s="81"/>
+      <c r="G31" s="81"/>
+      <c r="H31" s="81"/>
+      <c r="I31" s="81"/>
       <c r="J31" s="29"/>
       <c r="K31" s="29"/>
-      <c r="L31" s="80" t="s">
-        <v>1212</v>
-      </c>
-      <c r="M31" s="80"/>
-      <c r="N31" s="80"/>
-      <c r="O31" s="80"/>
-      <c r="P31" s="80"/>
-      <c r="Q31" s="80"/>
-      <c r="R31" s="80"/>
-      <c r="S31" s="80"/>
+      <c r="L31" s="75" t="s">
+        <v>1211</v>
+      </c>
+      <c r="M31" s="75"/>
+      <c r="N31" s="75"/>
+      <c r="O31" s="75"/>
+      <c r="P31" s="75"/>
+      <c r="Q31" s="75"/>
+      <c r="R31" s="75"/>
+      <c r="S31" s="75"/>
       <c r="T31" s="29"/>
       <c r="U31" s="29"/>
-      <c r="V31" s="80" t="s">
-        <v>1213</v>
-      </c>
-      <c r="W31" s="81"/>
-      <c r="X31" s="81"/>
-      <c r="Y31" s="81"/>
-      <c r="Z31" s="81"/>
-      <c r="AA31" s="81"/>
-      <c r="AB31" s="81"/>
-      <c r="AC31" s="81"/>
+      <c r="V31" s="75" t="s">
+        <v>1212</v>
+      </c>
+      <c r="W31" s="83"/>
+      <c r="X31" s="83"/>
+      <c r="Y31" s="83"/>
+      <c r="Z31" s="83"/>
+      <c r="AA31" s="83"/>
+      <c r="AB31" s="83"/>
+      <c r="AC31" s="83"/>
     </row>
     <row r="32" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="29"/>
@@ -14129,68 +14129,68 @@
       <c r="I32" s="29"/>
       <c r="J32" s="29"/>
       <c r="K32" s="29"/>
-      <c r="L32" s="80"/>
-      <c r="M32" s="80"/>
-      <c r="N32" s="80"/>
-      <c r="O32" s="80"/>
-      <c r="P32" s="80"/>
-      <c r="Q32" s="80"/>
-      <c r="R32" s="80"/>
-      <c r="S32" s="80"/>
+      <c r="L32" s="75"/>
+      <c r="M32" s="75"/>
+      <c r="N32" s="75"/>
+      <c r="O32" s="75"/>
+      <c r="P32" s="75"/>
+      <c r="Q32" s="75"/>
+      <c r="R32" s="75"/>
+      <c r="S32" s="75"/>
       <c r="T32" s="29"/>
       <c r="U32" s="29"/>
-      <c r="V32" s="81"/>
-      <c r="W32" s="81"/>
-      <c r="X32" s="81"/>
-      <c r="Y32" s="81"/>
-      <c r="Z32" s="81"/>
-      <c r="AA32" s="81"/>
-      <c r="AB32" s="81"/>
-      <c r="AC32" s="81"/>
+      <c r="V32" s="83"/>
+      <c r="W32" s="83"/>
+      <c r="X32" s="83"/>
+      <c r="Y32" s="83"/>
+      <c r="Z32" s="83"/>
+      <c r="AA32" s="83"/>
+      <c r="AB32" s="83"/>
+      <c r="AC32" s="83"/>
     </row>
     <row r="33" spans="1:29" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="29"/>
-      <c r="B33" s="77" t="s">
-        <v>1214</v>
-      </c>
-      <c r="C33" s="77"/>
-      <c r="D33" s="77"/>
-      <c r="E33" s="77"/>
-      <c r="F33" s="77"/>
-      <c r="G33" s="77"/>
-      <c r="H33" s="77"/>
-      <c r="I33" s="77"/>
+      <c r="B33" s="78" t="s">
+        <v>1213</v>
+      </c>
+      <c r="C33" s="78"/>
+      <c r="D33" s="78"/>
+      <c r="E33" s="78"/>
+      <c r="F33" s="78"/>
+      <c r="G33" s="78"/>
+      <c r="H33" s="78"/>
+      <c r="I33" s="78"/>
       <c r="J33" s="29"/>
       <c r="K33" s="29"/>
-      <c r="L33" s="80"/>
-      <c r="M33" s="80"/>
-      <c r="N33" s="80"/>
-      <c r="O33" s="80"/>
-      <c r="P33" s="80"/>
-      <c r="Q33" s="80"/>
-      <c r="R33" s="80"/>
-      <c r="S33" s="80"/>
+      <c r="L33" s="75"/>
+      <c r="M33" s="75"/>
+      <c r="N33" s="75"/>
+      <c r="O33" s="75"/>
+      <c r="P33" s="75"/>
+      <c r="Q33" s="75"/>
+      <c r="R33" s="75"/>
+      <c r="S33" s="75"/>
       <c r="T33" s="29"/>
       <c r="U33" s="29"/>
-      <c r="V33" s="81"/>
-      <c r="W33" s="81"/>
-      <c r="X33" s="81"/>
-      <c r="Y33" s="81"/>
-      <c r="Z33" s="81"/>
-      <c r="AA33" s="81"/>
-      <c r="AB33" s="81"/>
-      <c r="AC33" s="81"/>
+      <c r="V33" s="83"/>
+      <c r="W33" s="83"/>
+      <c r="X33" s="83"/>
+      <c r="Y33" s="83"/>
+      <c r="Z33" s="83"/>
+      <c r="AA33" s="83"/>
+      <c r="AB33" s="83"/>
+      <c r="AC33" s="83"/>
     </row>
     <row r="34" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="29"/>
-      <c r="B34" s="77"/>
-      <c r="C34" s="77"/>
-      <c r="D34" s="77"/>
-      <c r="E34" s="77"/>
-      <c r="F34" s="77"/>
-      <c r="G34" s="77"/>
-      <c r="H34" s="77"/>
-      <c r="I34" s="77"/>
+      <c r="B34" s="78"/>
+      <c r="C34" s="78"/>
+      <c r="D34" s="78"/>
+      <c r="E34" s="78"/>
+      <c r="F34" s="78"/>
+      <c r="G34" s="78"/>
+      <c r="H34" s="78"/>
+      <c r="I34" s="78"/>
       <c r="J34" s="29"/>
       <c r="K34" s="29"/>
       <c r="L34" s="29"/>
@@ -14224,28 +14224,28 @@
       <c r="I35" s="29"/>
       <c r="J35" s="29"/>
       <c r="K35" s="29"/>
-      <c r="L35" s="80" t="s">
-        <v>1215</v>
-      </c>
-      <c r="M35" s="80"/>
-      <c r="N35" s="80"/>
-      <c r="O35" s="80"/>
-      <c r="P35" s="80"/>
-      <c r="Q35" s="80"/>
-      <c r="R35" s="80"/>
-      <c r="S35" s="80"/>
+      <c r="L35" s="75" t="s">
+        <v>1214</v>
+      </c>
+      <c r="M35" s="75"/>
+      <c r="N35" s="75"/>
+      <c r="O35" s="75"/>
+      <c r="P35" s="75"/>
+      <c r="Q35" s="75"/>
+      <c r="R35" s="75"/>
+      <c r="S35" s="75"/>
       <c r="T35" s="29"/>
       <c r="U35" s="29"/>
-      <c r="V35" s="77" t="s">
-        <v>1216</v>
-      </c>
-      <c r="W35" s="77"/>
-      <c r="X35" s="77"/>
-      <c r="Y35" s="77"/>
-      <c r="Z35" s="77"/>
-      <c r="AA35" s="77"/>
-      <c r="AB35" s="77"/>
-      <c r="AC35" s="77"/>
+      <c r="V35" s="78" t="s">
+        <v>1215</v>
+      </c>
+      <c r="W35" s="78"/>
+      <c r="X35" s="78"/>
+      <c r="Y35" s="78"/>
+      <c r="Z35" s="78"/>
+      <c r="AA35" s="78"/>
+      <c r="AB35" s="78"/>
+      <c r="AC35" s="78"/>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A36" s="29"/>
@@ -14259,24 +14259,24 @@
       <c r="I36" s="29"/>
       <c r="J36" s="29"/>
       <c r="K36" s="29"/>
-      <c r="L36" s="80"/>
-      <c r="M36" s="80"/>
-      <c r="N36" s="80"/>
-      <c r="O36" s="80"/>
-      <c r="P36" s="80"/>
-      <c r="Q36" s="80"/>
-      <c r="R36" s="80"/>
-      <c r="S36" s="80"/>
+      <c r="L36" s="75"/>
+      <c r="M36" s="75"/>
+      <c r="N36" s="75"/>
+      <c r="O36" s="75"/>
+      <c r="P36" s="75"/>
+      <c r="Q36" s="75"/>
+      <c r="R36" s="75"/>
+      <c r="S36" s="75"/>
       <c r="T36" s="29"/>
       <c r="U36" s="29"/>
-      <c r="V36" s="77"/>
-      <c r="W36" s="77"/>
-      <c r="X36" s="77"/>
-      <c r="Y36" s="77"/>
-      <c r="Z36" s="77"/>
-      <c r="AA36" s="77"/>
-      <c r="AB36" s="77"/>
-      <c r="AC36" s="77"/>
+      <c r="V36" s="78"/>
+      <c r="W36" s="78"/>
+      <c r="X36" s="78"/>
+      <c r="Y36" s="78"/>
+      <c r="Z36" s="78"/>
+      <c r="AA36" s="78"/>
+      <c r="AB36" s="78"/>
+      <c r="AC36" s="78"/>
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A37" s="29"/>
@@ -14290,14 +14290,14 @@
       <c r="I37" s="29"/>
       <c r="J37" s="29"/>
       <c r="K37" s="29"/>
-      <c r="L37" s="80"/>
-      <c r="M37" s="80"/>
-      <c r="N37" s="80"/>
-      <c r="O37" s="80"/>
-      <c r="P37" s="80"/>
-      <c r="Q37" s="80"/>
-      <c r="R37" s="80"/>
-      <c r="S37" s="80"/>
+      <c r="L37" s="75"/>
+      <c r="M37" s="75"/>
+      <c r="N37" s="75"/>
+      <c r="O37" s="75"/>
+      <c r="P37" s="75"/>
+      <c r="Q37" s="75"/>
+      <c r="R37" s="75"/>
+      <c r="S37" s="75"/>
       <c r="T37" s="29"/>
       <c r="U37" s="29"/>
       <c r="V37" s="29"/>
@@ -14321,26 +14321,26 @@
       <c r="I38" s="29"/>
       <c r="J38" s="29"/>
       <c r="K38" s="29"/>
-      <c r="L38" s="80"/>
-      <c r="M38" s="80"/>
-      <c r="N38" s="80"/>
-      <c r="O38" s="80"/>
-      <c r="P38" s="80"/>
-      <c r="Q38" s="80"/>
-      <c r="R38" s="80"/>
-      <c r="S38" s="80"/>
+      <c r="L38" s="75"/>
+      <c r="M38" s="75"/>
+      <c r="N38" s="75"/>
+      <c r="O38" s="75"/>
+      <c r="P38" s="75"/>
+      <c r="Q38" s="75"/>
+      <c r="R38" s="75"/>
+      <c r="S38" s="75"/>
       <c r="T38" s="29"/>
       <c r="U38" s="29"/>
-      <c r="V38" s="78" t="s">
-        <v>1209</v>
-      </c>
-      <c r="W38" s="78"/>
-      <c r="X38" s="78"/>
-      <c r="Y38" s="78"/>
-      <c r="Z38" s="78"/>
-      <c r="AA38" s="78"/>
-      <c r="AB38" s="78"/>
-      <c r="AC38" s="78"/>
+      <c r="V38" s="84" t="s">
+        <v>1208</v>
+      </c>
+      <c r="W38" s="84"/>
+      <c r="X38" s="84"/>
+      <c r="Y38" s="84"/>
+      <c r="Z38" s="84"/>
+      <c r="AA38" s="84"/>
+      <c r="AB38" s="84"/>
+      <c r="AC38" s="84"/>
     </row>
     <row r="39" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A39" s="29"/>
@@ -14354,26 +14354,26 @@
       <c r="I39" s="29"/>
       <c r="J39" s="29"/>
       <c r="K39" s="29"/>
-      <c r="L39" s="80" t="s">
-        <v>1217</v>
-      </c>
-      <c r="M39" s="80"/>
-      <c r="N39" s="80"/>
-      <c r="O39" s="80"/>
-      <c r="P39" s="80"/>
-      <c r="Q39" s="80"/>
-      <c r="R39" s="80"/>
-      <c r="S39" s="80"/>
+      <c r="L39" s="75" t="s">
+        <v>1216</v>
+      </c>
+      <c r="M39" s="75"/>
+      <c r="N39" s="75"/>
+      <c r="O39" s="75"/>
+      <c r="P39" s="75"/>
+      <c r="Q39" s="75"/>
+      <c r="R39" s="75"/>
+      <c r="S39" s="75"/>
       <c r="T39" s="29"/>
       <c r="U39" s="29"/>
-      <c r="V39" s="78"/>
-      <c r="W39" s="78"/>
-      <c r="X39" s="78"/>
-      <c r="Y39" s="78"/>
-      <c r="Z39" s="78"/>
-      <c r="AA39" s="78"/>
-      <c r="AB39" s="78"/>
-      <c r="AC39" s="78"/>
+      <c r="V39" s="84"/>
+      <c r="W39" s="84"/>
+      <c r="X39" s="84"/>
+      <c r="Y39" s="84"/>
+      <c r="Z39" s="84"/>
+      <c r="AA39" s="84"/>
+      <c r="AB39" s="84"/>
+      <c r="AC39" s="84"/>
     </row>
     <row r="40" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A40" s="29"/>
@@ -14387,14 +14387,14 @@
       <c r="I40" s="29"/>
       <c r="J40" s="29"/>
       <c r="K40" s="29"/>
-      <c r="L40" s="80"/>
-      <c r="M40" s="80"/>
-      <c r="N40" s="80"/>
-      <c r="O40" s="80"/>
-      <c r="P40" s="80"/>
-      <c r="Q40" s="80"/>
-      <c r="R40" s="80"/>
-      <c r="S40" s="80"/>
+      <c r="L40" s="75"/>
+      <c r="M40" s="75"/>
+      <c r="N40" s="75"/>
+      <c r="O40" s="75"/>
+      <c r="P40" s="75"/>
+      <c r="Q40" s="75"/>
+      <c r="R40" s="75"/>
+      <c r="S40" s="75"/>
       <c r="T40" s="29"/>
       <c r="U40" s="29"/>
       <c r="V40" s="29"/>
@@ -14418,28 +14418,28 @@
       <c r="I41" s="29"/>
       <c r="J41" s="29"/>
       <c r="K41" s="29"/>
-      <c r="L41" s="80" t="s">
-        <v>1218</v>
-      </c>
-      <c r="M41" s="80"/>
-      <c r="N41" s="80"/>
-      <c r="O41" s="80"/>
-      <c r="P41" s="80"/>
-      <c r="Q41" s="80"/>
-      <c r="R41" s="80"/>
-      <c r="S41" s="80"/>
+      <c r="L41" s="75" t="s">
+        <v>1217</v>
+      </c>
+      <c r="M41" s="75"/>
+      <c r="N41" s="75"/>
+      <c r="O41" s="75"/>
+      <c r="P41" s="75"/>
+      <c r="Q41" s="75"/>
+      <c r="R41" s="75"/>
+      <c r="S41" s="75"/>
       <c r="T41" s="29"/>
       <c r="U41" s="29"/>
-      <c r="V41" s="80" t="s">
-        <v>1219</v>
-      </c>
-      <c r="W41" s="80"/>
-      <c r="X41" s="80"/>
-      <c r="Y41" s="80"/>
-      <c r="Z41" s="80"/>
-      <c r="AA41" s="80"/>
-      <c r="AB41" s="80"/>
-      <c r="AC41" s="80"/>
+      <c r="V41" s="75" t="s">
+        <v>1218</v>
+      </c>
+      <c r="W41" s="75"/>
+      <c r="X41" s="75"/>
+      <c r="Y41" s="75"/>
+      <c r="Z41" s="75"/>
+      <c r="AA41" s="75"/>
+      <c r="AB41" s="75"/>
+      <c r="AC41" s="75"/>
     </row>
     <row r="42" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="29"/>
@@ -14453,24 +14453,24 @@
       <c r="I42" s="29"/>
       <c r="J42" s="29"/>
       <c r="K42" s="29"/>
-      <c r="L42" s="80"/>
-      <c r="M42" s="80"/>
-      <c r="N42" s="80"/>
-      <c r="O42" s="80"/>
-      <c r="P42" s="80"/>
-      <c r="Q42" s="80"/>
-      <c r="R42" s="80"/>
-      <c r="S42" s="80"/>
+      <c r="L42" s="75"/>
+      <c r="M42" s="75"/>
+      <c r="N42" s="75"/>
+      <c r="O42" s="75"/>
+      <c r="P42" s="75"/>
+      <c r="Q42" s="75"/>
+      <c r="R42" s="75"/>
+      <c r="S42" s="75"/>
       <c r="T42" s="29"/>
       <c r="U42" s="29"/>
-      <c r="V42" s="80"/>
-      <c r="W42" s="80"/>
-      <c r="X42" s="80"/>
-      <c r="Y42" s="80"/>
-      <c r="Z42" s="80"/>
-      <c r="AA42" s="80"/>
-      <c r="AB42" s="80"/>
-      <c r="AC42" s="80"/>
+      <c r="V42" s="75"/>
+      <c r="W42" s="75"/>
+      <c r="X42" s="75"/>
+      <c r="Y42" s="75"/>
+      <c r="Z42" s="75"/>
+      <c r="AA42" s="75"/>
+      <c r="AB42" s="75"/>
+      <c r="AC42" s="75"/>
     </row>
     <row r="43" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="29"/>
@@ -14484,26 +14484,26 @@
       <c r="I43" s="29"/>
       <c r="J43" s="29"/>
       <c r="K43" s="29"/>
-      <c r="L43" s="78" t="s">
-        <v>1220</v>
-      </c>
-      <c r="M43" s="78"/>
-      <c r="N43" s="78"/>
-      <c r="O43" s="78"/>
-      <c r="P43" s="78"/>
-      <c r="Q43" s="78"/>
-      <c r="R43" s="78"/>
-      <c r="S43" s="78"/>
+      <c r="L43" s="84" t="s">
+        <v>1219</v>
+      </c>
+      <c r="M43" s="84"/>
+      <c r="N43" s="84"/>
+      <c r="O43" s="84"/>
+      <c r="P43" s="84"/>
+      <c r="Q43" s="84"/>
+      <c r="R43" s="84"/>
+      <c r="S43" s="84"/>
       <c r="T43" s="29"/>
       <c r="U43" s="29"/>
-      <c r="V43" s="80"/>
-      <c r="W43" s="80"/>
-      <c r="X43" s="80"/>
-      <c r="Y43" s="80"/>
-      <c r="Z43" s="80"/>
-      <c r="AA43" s="80"/>
-      <c r="AB43" s="80"/>
-      <c r="AC43" s="80"/>
+      <c r="V43" s="75"/>
+      <c r="W43" s="75"/>
+      <c r="X43" s="75"/>
+      <c r="Y43" s="75"/>
+      <c r="Z43" s="75"/>
+      <c r="AA43" s="75"/>
+      <c r="AB43" s="75"/>
+      <c r="AC43" s="75"/>
     </row>
     <row r="44" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="29"/>
@@ -14517,26 +14517,26 @@
       <c r="I44" s="29"/>
       <c r="J44" s="29"/>
       <c r="K44" s="29"/>
-      <c r="L44" s="78"/>
-      <c r="M44" s="78"/>
-      <c r="N44" s="78"/>
-      <c r="O44" s="78"/>
-      <c r="P44" s="78"/>
-      <c r="Q44" s="78"/>
-      <c r="R44" s="78"/>
-      <c r="S44" s="78"/>
+      <c r="L44" s="84"/>
+      <c r="M44" s="84"/>
+      <c r="N44" s="84"/>
+      <c r="O44" s="84"/>
+      <c r="P44" s="84"/>
+      <c r="Q44" s="84"/>
+      <c r="R44" s="84"/>
+      <c r="S44" s="84"/>
       <c r="T44" s="29"/>
       <c r="U44" s="29"/>
-      <c r="V44" s="77" t="s">
-        <v>1221</v>
-      </c>
-      <c r="W44" s="77"/>
-      <c r="X44" s="77"/>
-      <c r="Y44" s="77"/>
-      <c r="Z44" s="77"/>
-      <c r="AA44" s="77"/>
-      <c r="AB44" s="77"/>
-      <c r="AC44" s="77"/>
+      <c r="V44" s="78" t="s">
+        <v>1220</v>
+      </c>
+      <c r="W44" s="78"/>
+      <c r="X44" s="78"/>
+      <c r="Y44" s="78"/>
+      <c r="Z44" s="78"/>
+      <c r="AA44" s="78"/>
+      <c r="AB44" s="78"/>
+      <c r="AC44" s="78"/>
     </row>
     <row r="45" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A45" s="29"/>
@@ -14550,24 +14550,24 @@
       <c r="I45" s="29"/>
       <c r="J45" s="29"/>
       <c r="K45" s="29"/>
-      <c r="L45" s="78"/>
-      <c r="M45" s="78"/>
-      <c r="N45" s="78"/>
-      <c r="O45" s="78"/>
-      <c r="P45" s="78"/>
-      <c r="Q45" s="78"/>
-      <c r="R45" s="78"/>
-      <c r="S45" s="78"/>
+      <c r="L45" s="84"/>
+      <c r="M45" s="84"/>
+      <c r="N45" s="84"/>
+      <c r="O45" s="84"/>
+      <c r="P45" s="84"/>
+      <c r="Q45" s="84"/>
+      <c r="R45" s="84"/>
+      <c r="S45" s="84"/>
       <c r="T45" s="29"/>
       <c r="U45" s="29"/>
-      <c r="V45" s="77"/>
-      <c r="W45" s="77"/>
-      <c r="X45" s="77"/>
-      <c r="Y45" s="77"/>
-      <c r="Z45" s="77"/>
-      <c r="AA45" s="77"/>
-      <c r="AB45" s="77"/>
-      <c r="AC45" s="77"/>
+      <c r="V45" s="78"/>
+      <c r="W45" s="78"/>
+      <c r="X45" s="78"/>
+      <c r="Y45" s="78"/>
+      <c r="Z45" s="78"/>
+      <c r="AA45" s="78"/>
+      <c r="AB45" s="78"/>
+      <c r="AC45" s="78"/>
     </row>
     <row r="46" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="29"/>
@@ -14581,16 +14581,16 @@
       <c r="I46" s="29"/>
       <c r="J46" s="29"/>
       <c r="K46" s="29"/>
-      <c r="L46" s="80" t="s">
-        <v>1222</v>
-      </c>
-      <c r="M46" s="80"/>
-      <c r="N46" s="80"/>
-      <c r="O46" s="80"/>
-      <c r="P46" s="80"/>
-      <c r="Q46" s="80"/>
-      <c r="R46" s="80"/>
-      <c r="S46" s="80"/>
+      <c r="L46" s="75" t="s">
+        <v>1221</v>
+      </c>
+      <c r="M46" s="75"/>
+      <c r="N46" s="75"/>
+      <c r="O46" s="75"/>
+      <c r="P46" s="75"/>
+      <c r="Q46" s="75"/>
+      <c r="R46" s="75"/>
+      <c r="S46" s="75"/>
       <c r="T46" s="29"/>
       <c r="U46" s="29"/>
       <c r="V46" s="29"/>
@@ -14604,26 +14604,26 @@
     </row>
     <row r="47" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="29"/>
-      <c r="B47" s="77" t="s">
-        <v>1223</v>
-      </c>
-      <c r="C47" s="77"/>
-      <c r="D47" s="77"/>
-      <c r="E47" s="77"/>
-      <c r="F47" s="77"/>
-      <c r="G47" s="77"/>
-      <c r="H47" s="77"/>
-      <c r="I47" s="77"/>
+      <c r="B47" s="78" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C47" s="78"/>
+      <c r="D47" s="78"/>
+      <c r="E47" s="78"/>
+      <c r="F47" s="78"/>
+      <c r="G47" s="78"/>
+      <c r="H47" s="78"/>
+      <c r="I47" s="78"/>
       <c r="J47" s="29"/>
       <c r="K47" s="29"/>
-      <c r="L47" s="80"/>
-      <c r="M47" s="80"/>
-      <c r="N47" s="80"/>
-      <c r="O47" s="80"/>
-      <c r="P47" s="80"/>
-      <c r="Q47" s="80"/>
-      <c r="R47" s="80"/>
-      <c r="S47" s="80"/>
+      <c r="L47" s="75"/>
+      <c r="M47" s="75"/>
+      <c r="N47" s="75"/>
+      <c r="O47" s="75"/>
+      <c r="P47" s="75"/>
+      <c r="Q47" s="75"/>
+      <c r="R47" s="75"/>
+      <c r="S47" s="75"/>
       <c r="T47" s="29"/>
       <c r="U47" s="29"/>
       <c r="V47" s="29"/>
@@ -14637,24 +14637,24 @@
     </row>
     <row r="48" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="29"/>
-      <c r="B48" s="77"/>
-      <c r="C48" s="77"/>
-      <c r="D48" s="77"/>
-      <c r="E48" s="77"/>
-      <c r="F48" s="77"/>
-      <c r="G48" s="77"/>
-      <c r="H48" s="77"/>
-      <c r="I48" s="77"/>
+      <c r="B48" s="78"/>
+      <c r="C48" s="78"/>
+      <c r="D48" s="78"/>
+      <c r="E48" s="78"/>
+      <c r="F48" s="78"/>
+      <c r="G48" s="78"/>
+      <c r="H48" s="78"/>
+      <c r="I48" s="78"/>
       <c r="J48" s="29"/>
       <c r="K48" s="29"/>
-      <c r="L48" s="80"/>
-      <c r="M48" s="80"/>
-      <c r="N48" s="80"/>
-      <c r="O48" s="80"/>
-      <c r="P48" s="80"/>
-      <c r="Q48" s="80"/>
-      <c r="R48" s="80"/>
-      <c r="S48" s="80"/>
+      <c r="L48" s="75"/>
+      <c r="M48" s="75"/>
+      <c r="N48" s="75"/>
+      <c r="O48" s="75"/>
+      <c r="P48" s="75"/>
+      <c r="Q48" s="75"/>
+      <c r="R48" s="75"/>
+      <c r="S48" s="75"/>
       <c r="T48" s="29"/>
       <c r="U48" s="29"/>
       <c r="V48" s="29"/>
@@ -14668,14 +14668,14 @@
     </row>
     <row r="49" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="29"/>
-      <c r="B49" s="77"/>
-      <c r="C49" s="77"/>
-      <c r="D49" s="77"/>
-      <c r="E49" s="77"/>
-      <c r="F49" s="77"/>
-      <c r="G49" s="77"/>
-      <c r="H49" s="77"/>
-      <c r="I49" s="77"/>
+      <c r="B49" s="78"/>
+      <c r="C49" s="78"/>
+      <c r="D49" s="78"/>
+      <c r="E49" s="78"/>
+      <c r="F49" s="78"/>
+      <c r="G49" s="78"/>
+      <c r="H49" s="78"/>
+      <c r="I49" s="78"/>
       <c r="J49" s="29"/>
       <c r="K49" s="29"/>
       <c r="L49" s="29"/>
@@ -14699,14 +14699,14 @@
     </row>
     <row r="50" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A50" s="29"/>
-      <c r="B50" s="77"/>
-      <c r="C50" s="77"/>
-      <c r="D50" s="77"/>
-      <c r="E50" s="77"/>
-      <c r="F50" s="77"/>
-      <c r="G50" s="77"/>
-      <c r="H50" s="77"/>
-      <c r="I50" s="77"/>
+      <c r="B50" s="78"/>
+      <c r="C50" s="78"/>
+      <c r="D50" s="78"/>
+      <c r="E50" s="78"/>
+      <c r="F50" s="78"/>
+      <c r="G50" s="78"/>
+      <c r="H50" s="78"/>
+      <c r="I50" s="78"/>
       <c r="J50" s="29"/>
       <c r="K50" s="29"/>
       <c r="L50" s="29"/>
@@ -14730,14 +14730,14 @@
     </row>
     <row r="51" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A51" s="29"/>
-      <c r="B51" s="77"/>
-      <c r="C51" s="77"/>
-      <c r="D51" s="77"/>
-      <c r="E51" s="77"/>
-      <c r="F51" s="77"/>
-      <c r="G51" s="77"/>
-      <c r="H51" s="77"/>
-      <c r="I51" s="77"/>
+      <c r="B51" s="78"/>
+      <c r="C51" s="78"/>
+      <c r="D51" s="78"/>
+      <c r="E51" s="78"/>
+      <c r="F51" s="78"/>
+      <c r="G51" s="78"/>
+      <c r="H51" s="78"/>
+      <c r="I51" s="78"/>
       <c r="J51" s="29"/>
       <c r="K51" s="29"/>
       <c r="L51" s="29"/>
@@ -15892,18 +15892,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="Ni3oRhRFSHLqcHPeDMM9oJPhO6WfMxTCuA0QUr0aYxZ5GIVg5SnJ0DmCKugqbXaRKsIRpp0xaviZSFtXtsEQYA==" saltValue="uU6zNIz4+Gs4uisLnne5sQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="27">
-    <mergeCell ref="L20:S21"/>
-    <mergeCell ref="B4:I4"/>
-    <mergeCell ref="V4:AC4"/>
-    <mergeCell ref="B5:I5"/>
-    <mergeCell ref="V5:AC5"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="V7:AC7"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="V8:AC8"/>
-    <mergeCell ref="V10:AC10"/>
-    <mergeCell ref="L16:S17"/>
-    <mergeCell ref="L18:S18"/>
     <mergeCell ref="B47:I51"/>
     <mergeCell ref="L23:S24"/>
     <mergeCell ref="B31:I31"/>
@@ -15919,6 +15907,18 @@
     <mergeCell ref="L43:S45"/>
     <mergeCell ref="V44:AC45"/>
     <mergeCell ref="L46:S48"/>
+    <mergeCell ref="L20:S21"/>
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="V4:AC4"/>
+    <mergeCell ref="B5:I5"/>
+    <mergeCell ref="V5:AC5"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="V7:AC7"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="V8:AC8"/>
+    <mergeCell ref="V10:AC10"/>
+    <mergeCell ref="L16:S17"/>
+    <mergeCell ref="L18:S18"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1" xr:uid="{5E7C7A05-D050-4790-AD5A-2C904F987D3F}"/>
@@ -15943,79 +15943,79 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.33203125" style="62" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="64" customWidth="1"/>
-    <col min="3" max="3" width="87.1640625" style="62" customWidth="1"/>
-    <col min="4" max="4" width="49.5" style="61" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.83203125" style="62"/>
+    <col min="1" max="1" width="38.33203125" style="60" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" style="62" customWidth="1"/>
+    <col min="3" max="3" width="87.1640625" style="60" customWidth="1"/>
+    <col min="4" max="4" width="49.5" style="59" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="60"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="57" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:4" s="55" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="55" t="s">
         <v>1162</v>
       </c>
-      <c r="B1" s="58" t="s">
-        <v>1194</v>
-      </c>
-      <c r="C1" s="57" t="s">
+      <c r="B1" s="56" t="s">
+        <v>1193</v>
+      </c>
+      <c r="C1" s="55" t="s">
         <v>1163</v>
       </c>
-      <c r="D1" s="59" t="s">
-        <v>1193</v>
+      <c r="D1" s="57" t="s">
+        <v>1192</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="52" t="s">
         <v>1164</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="60" t="s">
+      <c r="C2" s="58" t="s">
         <v>1165</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="52" t="s">
         <v>1166</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="58" t="s">
         <v>1167</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="52" t="s">
         <v>1168</v>
       </c>
-      <c r="B4" s="55" t="s">
+      <c r="B4" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="58" t="s">
         <v>1169</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="60" t="s">
+      <c r="C5" s="58" t="s">
         <v>1170</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="60" t="s">
+      <c r="C6" s="58" t="s">
         <v>1171</v>
       </c>
     </row>
@@ -16023,8 +16023,8 @@
       <c r="A7" s="32" t="s">
         <v>1172</v>
       </c>
-      <c r="B7" s="56"/>
-      <c r="C7" s="62" t="s">
+      <c r="B7" s="54"/>
+      <c r="C7" s="60" t="s">
         <v>1173</v>
       </c>
     </row>
@@ -16032,8 +16032,8 @@
       <c r="A8" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="B8" s="56"/>
-      <c r="C8" s="62" t="s">
+      <c r="B8" s="54"/>
+      <c r="C8" s="60" t="s">
         <v>1174</v>
       </c>
     </row>
@@ -16041,65 +16041,65 @@
       <c r="A9" s="32" t="s">
         <v>1175</v>
       </c>
-      <c r="B9" s="56"/>
-      <c r="C9" s="62" t="s">
+      <c r="B9" s="54"/>
+      <c r="C9" s="60" t="s">
         <v>1176</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A10" s="54" t="s">
+      <c r="A10" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="55" t="s">
+      <c r="B10" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="63" t="s">
+      <c r="C10" s="61" t="s">
         <v>1177</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="54" t="s">
+      <c r="A11" s="52" t="s">
         <v>408</v>
       </c>
-      <c r="B11" s="55" t="s">
+      <c r="B11" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="60" t="s">
+      <c r="C11" s="58" t="s">
         <v>1178</v>
       </c>
-      <c r="D11" s="61" t="s">
-        <v>1195</v>
+      <c r="D11" s="59" t="s">
+        <v>1194</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="32" t="s">
         <v>409</v>
       </c>
-      <c r="B12" s="56"/>
-      <c r="C12" s="62" t="s">
+      <c r="B12" s="54"/>
+      <c r="C12" s="60" t="s">
         <v>1179</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="54" t="s">
+      <c r="A13" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="55" t="s">
+      <c r="B13" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="60" t="s">
+      <c r="C13" s="58" t="s">
         <v>1180</v>
       </c>
-      <c r="D13" s="61" t="s">
-        <v>1196</v>
+      <c r="D13" s="59" t="s">
+        <v>1195</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="56"/>
-      <c r="C14" s="62" t="s">
+      <c r="B14" s="54"/>
+      <c r="C14" s="60" t="s">
         <v>1180</v>
       </c>
     </row>
@@ -16107,8 +16107,8 @@
       <c r="A15" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="56"/>
-      <c r="C15" s="62" t="s">
+      <c r="B15" s="54"/>
+      <c r="C15" s="60" t="s">
         <v>1180</v>
       </c>
     </row>
@@ -16116,8 +16116,8 @@
       <c r="A16" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="56"/>
-      <c r="C16" s="62" t="s">
+      <c r="B16" s="54"/>
+      <c r="C16" s="60" t="s">
         <v>1180</v>
       </c>
     </row>
@@ -16125,8 +16125,8 @@
       <c r="A17" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="B17" s="56"/>
-      <c r="C17" s="62" t="s">
+      <c r="B17" s="54"/>
+      <c r="C17" s="60" t="s">
         <v>1180</v>
       </c>
     </row>
@@ -16134,8 +16134,8 @@
       <c r="A18" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="56"/>
-      <c r="C18" s="62" t="s">
+      <c r="B18" s="54"/>
+      <c r="C18" s="60" t="s">
         <v>1180</v>
       </c>
     </row>
@@ -16143,8 +16143,8 @@
       <c r="A19" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="56"/>
-      <c r="C19" s="62" t="s">
+      <c r="B19" s="54"/>
+      <c r="C19" s="60" t="s">
         <v>1180</v>
       </c>
     </row>
@@ -16152,8 +16152,8 @@
       <c r="A20" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="B20" s="56"/>
-      <c r="C20" s="62" t="s">
+      <c r="B20" s="54"/>
+      <c r="C20" s="60" t="s">
         <v>1180</v>
       </c>
     </row>
@@ -16161,22 +16161,22 @@
       <c r="A21" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="56"/>
-      <c r="C21" s="62" t="s">
+      <c r="B21" s="54"/>
+      <c r="C21" s="60" t="s">
         <v>1181</v>
       </c>
-      <c r="D21" s="61" t="s">
-        <v>1197</v>
+      <c r="D21" s="59" t="s">
+        <v>1196</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="54" t="s">
+      <c r="A22" s="52" t="s">
         <v>1182</v>
       </c>
-      <c r="B22" s="55" t="s">
+      <c r="B22" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="60" t="s">
+      <c r="C22" s="58" t="s">
         <v>1183</v>
       </c>
     </row>
@@ -16194,8 +16194,8 @@
   </sheetPr>
   <dimension ref="A1:AF63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16233,22 +16233,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="51" t="s">
         <v>1105</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="51" t="s">
         <v>1106</v>
       </c>
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="51" t="s">
         <v>1107</v>
       </c>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="51" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="25" t="s">
         <v>1108</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="51" t="s">
         <v>55</v>
       </c>
       <c r="G1" s="25" t="s">
@@ -16260,71 +16260,71 @@
       <c r="I1" s="25" t="s">
         <v>1184</v>
       </c>
-      <c r="J1" s="53" t="s">
+      <c r="J1" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="K1" s="53" t="s">
+      <c r="K1" s="51" t="s">
         <v>408</v>
       </c>
       <c r="L1" s="34" t="s">
         <v>409</v>
       </c>
-      <c r="M1" s="73" t="s">
+      <c r="M1" s="71" t="s">
         <v>1110</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>1245</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>1246</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>1247</v>
-      </c>
-      <c r="P1" s="71" t="s">
+      <c r="P1" s="69" t="s">
+        <v>1229</v>
+      </c>
+      <c r="Q1" s="26" t="s">
         <v>1230</v>
       </c>
-      <c r="Q1" s="26" t="s">
+      <c r="R1" s="33" t="s">
         <v>1231</v>
       </c>
-      <c r="R1" s="33" t="s">
+      <c r="S1" s="28" t="s">
         <v>1232</v>
       </c>
-      <c r="S1" s="28" t="s">
+      <c r="T1" s="36" t="s">
         <v>1233</v>
       </c>
-      <c r="T1" s="36" t="s">
+      <c r="U1" s="28" t="s">
         <v>1234</v>
       </c>
-      <c r="U1" s="28" t="s">
+      <c r="V1" s="35" t="s">
         <v>1235</v>
       </c>
-      <c r="V1" s="35" t="s">
+      <c r="W1" s="28" t="s">
         <v>1236</v>
       </c>
-      <c r="W1" s="28" t="s">
+      <c r="X1" s="35" t="s">
         <v>1237</v>
       </c>
-      <c r="X1" s="35" t="s">
+      <c r="Y1" s="27" t="s">
         <v>1238</v>
       </c>
-      <c r="Y1" s="27" t="s">
+      <c r="Z1" s="35" t="s">
         <v>1239</v>
       </c>
-      <c r="Z1" s="35" t="s">
+      <c r="AA1" s="27" t="s">
         <v>1240</v>
       </c>
-      <c r="AA1" s="27" t="s">
+      <c r="AB1" s="35" t="s">
         <v>1241</v>
       </c>
-      <c r="AB1" s="35" t="s">
+      <c r="AC1" s="27" t="s">
         <v>1242</v>
       </c>
-      <c r="AC1" s="27" t="s">
+      <c r="AD1" s="35" t="s">
         <v>1243</v>
       </c>
-      <c r="AD1" s="35" t="s">
+      <c r="AE1" s="27" t="s">
         <v>1244</v>
-      </c>
-      <c r="AE1" s="27" t="s">
-        <v>1245</v>
       </c>
       <c r="AF1" s="35" t="s">
         <v>2</v>
@@ -16332,13 +16332,13 @@
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="38" t="s">
+        <v>1225</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C2" s="38" t="s">
         <v>1226</v>
-      </c>
-      <c r="B2" s="38" t="s">
-        <v>1226</v>
-      </c>
-      <c r="C2" s="39" t="s">
-        <v>1227</v>
       </c>
       <c r="D2" s="38" t="s">
         <v>6</v>
@@ -16363,15 +16363,15 @@
         <v>52</v>
       </c>
       <c r="K2" s="38" t="s">
-        <v>1261</v>
-      </c>
-      <c r="L2" s="70"/>
+        <v>1260</v>
+      </c>
+      <c r="L2" s="68"/>
       <c r="M2" s="38" t="s">
         <v>1111</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
-      <c r="P2" s="72" t="s">
+      <c r="P2" s="70" t="s">
         <v>13</v>
       </c>
       <c r="Q2" s="1" t="str">
@@ -16417,13 +16417,13 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>1229</v>
-      </c>
-      <c r="C3" s="39" t="s">
         <v>1228</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>1227</v>
       </c>
       <c r="D3" s="38" t="s">
         <v>11</v>
@@ -16445,18 +16445,18 @@
         <v/>
       </c>
       <c r="J3" s="38" t="s">
-        <v>1185</v>
+        <v>1262</v>
       </c>
       <c r="K3" s="38" t="s">
-        <v>1262</v>
-      </c>
-      <c r="L3" s="70"/>
+        <v>1261</v>
+      </c>
+      <c r="L3" s="68"/>
       <c r="M3" s="38" t="s">
         <v>1111</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
-      <c r="P3" s="72" t="s">
+      <c r="P3" s="70" t="s">
         <v>1158</v>
       </c>
       <c r="Q3" s="1" t="str">
@@ -16503,7 +16503,7 @@
     <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" s="38"/>
       <c r="B4" s="38"/>
-      <c r="C4" s="39"/>
+      <c r="C4" s="38"/>
       <c r="D4" s="38"/>
       <c r="E4" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D4,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D4,Region!$A$1:$B$9,2,FALSE))</f>
@@ -16521,11 +16521,11 @@
       </c>
       <c r="J4" s="38"/>
       <c r="K4" s="38"/>
-      <c r="L4" s="70"/>
+      <c r="L4" s="68"/>
       <c r="M4" s="38"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
-      <c r="P4" s="72"/>
+      <c r="P4" s="70"/>
       <c r="Q4" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P4,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P4,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -16570,7 +16570,7 @@
     <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A5" s="38"/>
       <c r="B5" s="38"/>
-      <c r="C5" s="39"/>
+      <c r="C5" s="38"/>
       <c r="D5" s="38"/>
       <c r="E5" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D5,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D5,Region!$A$1:$B$9,2,FALSE))</f>
@@ -16588,11 +16588,11 @@
       </c>
       <c r="J5" s="38"/>
       <c r="K5" s="38"/>
-      <c r="L5" s="70"/>
+      <c r="L5" s="68"/>
       <c r="M5" s="38"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
-      <c r="P5" s="72"/>
+      <c r="P5" s="70"/>
       <c r="Q5" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P5,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P5,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -16637,7 +16637,7 @@
     <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A6" s="38"/>
       <c r="B6" s="38"/>
-      <c r="C6" s="39"/>
+      <c r="C6" s="38"/>
       <c r="D6" s="38"/>
       <c r="E6" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D6,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D6,Region!$A$1:$B$9,2,FALSE))</f>
@@ -16655,11 +16655,11 @@
       </c>
       <c r="J6" s="38"/>
       <c r="K6" s="38"/>
-      <c r="L6" s="70"/>
+      <c r="L6" s="68"/>
       <c r="M6" s="38"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-      <c r="P6" s="72"/>
+      <c r="P6" s="70"/>
       <c r="Q6" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P6,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P6,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -16704,7 +16704,7 @@
     <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A7" s="38"/>
       <c r="B7" s="38"/>
-      <c r="C7" s="39"/>
+      <c r="C7" s="38"/>
       <c r="D7" s="38"/>
       <c r="E7" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D7,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D7,Region!$A$1:$B$9,2,FALSE))</f>
@@ -16722,11 +16722,11 @@
       </c>
       <c r="J7" s="38"/>
       <c r="K7" s="38"/>
-      <c r="L7" s="70"/>
+      <c r="L7" s="68"/>
       <c r="M7" s="38"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
-      <c r="P7" s="72"/>
+      <c r="P7" s="70"/>
       <c r="Q7" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P7,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P7,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -16771,7 +16771,7 @@
     <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A8" s="38"/>
       <c r="B8" s="38"/>
-      <c r="C8" s="39"/>
+      <c r="C8" s="38"/>
       <c r="D8" s="38"/>
       <c r="E8" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D8,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D8,Region!$A$1:$B$9,2,FALSE))</f>
@@ -16789,11 +16789,11 @@
       </c>
       <c r="J8" s="38"/>
       <c r="K8" s="38"/>
-      <c r="L8" s="70"/>
+      <c r="L8" s="68"/>
       <c r="M8" s="38"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
-      <c r="P8" s="72"/>
+      <c r="P8" s="70"/>
       <c r="Q8" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P8,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P8,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -16838,7 +16838,7 @@
     <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A9" s="38"/>
       <c r="B9" s="38"/>
-      <c r="C9" s="39"/>
+      <c r="C9" s="38"/>
       <c r="D9" s="38"/>
       <c r="E9" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D9,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D9,Region!$A$1:$B$9,2,FALSE))</f>
@@ -16856,11 +16856,11 @@
       </c>
       <c r="J9" s="38"/>
       <c r="K9" s="38"/>
-      <c r="L9" s="70"/>
+      <c r="L9" s="68"/>
       <c r="M9" s="38"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
-      <c r="P9" s="72"/>
+      <c r="P9" s="70"/>
       <c r="Q9" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P9,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P9,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -16905,7 +16905,7 @@
     <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A10" s="38"/>
       <c r="B10" s="38"/>
-      <c r="C10" s="39"/>
+      <c r="C10" s="38"/>
       <c r="D10" s="38"/>
       <c r="E10" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D10,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D10,Region!$A$1:$B$9,2,FALSE))</f>
@@ -16923,11 +16923,11 @@
       </c>
       <c r="J10" s="38"/>
       <c r="K10" s="38"/>
-      <c r="L10" s="70"/>
+      <c r="L10" s="68"/>
       <c r="M10" s="38"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
-      <c r="P10" s="72"/>
+      <c r="P10" s="70"/>
       <c r="Q10" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P10,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P10,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -16972,7 +16972,7 @@
     <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A11" s="38"/>
       <c r="B11" s="38"/>
-      <c r="C11" s="39"/>
+      <c r="C11" s="38"/>
       <c r="D11" s="38"/>
       <c r="E11" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D11,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D11,Region!$A$1:$B$9,2,FALSE))</f>
@@ -16990,11 +16990,11 @@
       </c>
       <c r="J11" s="38"/>
       <c r="K11" s="38"/>
-      <c r="L11" s="70"/>
+      <c r="L11" s="68"/>
       <c r="M11" s="38"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
-      <c r="P11" s="72"/>
+      <c r="P11" s="70"/>
       <c r="Q11" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P11,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P11,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -17039,7 +17039,7 @@
     <row r="12" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A12" s="38"/>
       <c r="B12" s="38"/>
-      <c r="C12" s="39"/>
+      <c r="C12" s="38"/>
       <c r="D12" s="38"/>
       <c r="E12" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D12,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D12,Region!$A$1:$B$9,2,FALSE))</f>
@@ -17057,11 +17057,11 @@
       </c>
       <c r="J12" s="38"/>
       <c r="K12" s="38"/>
-      <c r="L12" s="70"/>
+      <c r="L12" s="68"/>
       <c r="M12" s="38"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
-      <c r="P12" s="72"/>
+      <c r="P12" s="70"/>
       <c r="Q12" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P12,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P12,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -17106,7 +17106,7 @@
     <row r="13" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A13" s="38"/>
       <c r="B13" s="38"/>
-      <c r="C13" s="39"/>
+      <c r="C13" s="38"/>
       <c r="D13" s="38"/>
       <c r="E13" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D13,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D13,Region!$A$1:$B$9,2,FALSE))</f>
@@ -17124,11 +17124,11 @@
       </c>
       <c r="J13" s="38"/>
       <c r="K13" s="38"/>
-      <c r="L13" s="70"/>
+      <c r="L13" s="68"/>
       <c r="M13" s="38"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
-      <c r="P13" s="72"/>
+      <c r="P13" s="70"/>
       <c r="Q13" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P13,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P13,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -17173,7 +17173,7 @@
     <row r="14" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A14" s="38"/>
       <c r="B14" s="38"/>
-      <c r="C14" s="39"/>
+      <c r="C14" s="38"/>
       <c r="D14" s="38"/>
       <c r="E14" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D14,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D14,Region!$A$1:$B$9,2,FALSE))</f>
@@ -17191,11 +17191,11 @@
       </c>
       <c r="J14" s="38"/>
       <c r="K14" s="38"/>
-      <c r="L14" s="70"/>
+      <c r="L14" s="68"/>
       <c r="M14" s="38"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
-      <c r="P14" s="72"/>
+      <c r="P14" s="70"/>
       <c r="Q14" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P14,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P14,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -17240,7 +17240,7 @@
     <row r="15" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A15" s="38"/>
       <c r="B15" s="38"/>
-      <c r="C15" s="39"/>
+      <c r="C15" s="38"/>
       <c r="D15" s="38"/>
       <c r="E15" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D15,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D15,Region!$A$1:$B$9,2,FALSE))</f>
@@ -17258,11 +17258,11 @@
       </c>
       <c r="J15" s="38"/>
       <c r="K15" s="38"/>
-      <c r="L15" s="70"/>
+      <c r="L15" s="68"/>
       <c r="M15" s="38"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
-      <c r="P15" s="72"/>
+      <c r="P15" s="70"/>
       <c r="Q15" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P15,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P15,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -17307,7 +17307,7 @@
     <row r="16" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A16" s="38"/>
       <c r="B16" s="38"/>
-      <c r="C16" s="39"/>
+      <c r="C16" s="38"/>
       <c r="D16" s="38"/>
       <c r="E16" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D16,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D16,Region!$A$1:$B$9,2,FALSE))</f>
@@ -17325,11 +17325,11 @@
       </c>
       <c r="J16" s="38"/>
       <c r="K16" s="38"/>
-      <c r="L16" s="70"/>
+      <c r="L16" s="68"/>
       <c r="M16" s="38"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
-      <c r="P16" s="72"/>
+      <c r="P16" s="70"/>
       <c r="Q16" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P16,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P16,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -17374,7 +17374,7 @@
     <row r="17" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A17" s="38"/>
       <c r="B17" s="38"/>
-      <c r="C17" s="39"/>
+      <c r="C17" s="38"/>
       <c r="D17" s="38"/>
       <c r="E17" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D17,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D17,Region!$A$1:$B$9,2,FALSE))</f>
@@ -17392,11 +17392,11 @@
       </c>
       <c r="J17" s="38"/>
       <c r="K17" s="38"/>
-      <c r="L17" s="70"/>
+      <c r="L17" s="68"/>
       <c r="M17" s="38"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
-      <c r="P17" s="72"/>
+      <c r="P17" s="70"/>
       <c r="Q17" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P17,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P17,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -17441,7 +17441,7 @@
     <row r="18" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A18" s="38"/>
       <c r="B18" s="38"/>
-      <c r="C18" s="39"/>
+      <c r="C18" s="38"/>
       <c r="D18" s="38"/>
       <c r="E18" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D18,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D18,Region!$A$1:$B$9,2,FALSE))</f>
@@ -17459,11 +17459,11 @@
       </c>
       <c r="J18" s="38"/>
       <c r="K18" s="38"/>
-      <c r="L18" s="70"/>
+      <c r="L18" s="68"/>
       <c r="M18" s="38"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
-      <c r="P18" s="72"/>
+      <c r="P18" s="70"/>
       <c r="Q18" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P18,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P18,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -17508,7 +17508,7 @@
     <row r="19" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A19" s="38"/>
       <c r="B19" s="38"/>
-      <c r="C19" s="39"/>
+      <c r="C19" s="38"/>
       <c r="D19" s="38"/>
       <c r="E19" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D19,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D19,Region!$A$1:$B$9,2,FALSE))</f>
@@ -17526,11 +17526,11 @@
       </c>
       <c r="J19" s="38"/>
       <c r="K19" s="38"/>
-      <c r="L19" s="70"/>
+      <c r="L19" s="68"/>
       <c r="M19" s="38"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
-      <c r="P19" s="72"/>
+      <c r="P19" s="70"/>
       <c r="Q19" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P19,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P19,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -17575,7 +17575,7 @@
     <row r="20" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A20" s="38"/>
       <c r="B20" s="38"/>
-      <c r="C20" s="39"/>
+      <c r="C20" s="38"/>
       <c r="D20" s="38"/>
       <c r="E20" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D20,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D20,Region!$A$1:$B$9,2,FALSE))</f>
@@ -17593,11 +17593,11 @@
       </c>
       <c r="J20" s="38"/>
       <c r="K20" s="38"/>
-      <c r="L20" s="70"/>
+      <c r="L20" s="68"/>
       <c r="M20" s="38"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
-      <c r="P20" s="72"/>
+      <c r="P20" s="70"/>
       <c r="Q20" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P20,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P20,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -17642,7 +17642,7 @@
     <row r="21" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A21" s="38"/>
       <c r="B21" s="38"/>
-      <c r="C21" s="39"/>
+      <c r="C21" s="38"/>
       <c r="D21" s="38"/>
       <c r="E21" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D21,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D21,Region!$A$1:$B$9,2,FALSE))</f>
@@ -17660,11 +17660,11 @@
       </c>
       <c r="J21" s="38"/>
       <c r="K21" s="38"/>
-      <c r="L21" s="70"/>
+      <c r="L21" s="68"/>
       <c r="M21" s="38"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
-      <c r="P21" s="72"/>
+      <c r="P21" s="70"/>
       <c r="Q21" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P21,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P21,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -17709,7 +17709,7 @@
     <row r="22" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A22" s="38"/>
       <c r="B22" s="38"/>
-      <c r="C22" s="39"/>
+      <c r="C22" s="38"/>
       <c r="D22" s="38"/>
       <c r="E22" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D22,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D22,Region!$A$1:$B$9,2,FALSE))</f>
@@ -17727,11 +17727,11 @@
       </c>
       <c r="J22" s="38"/>
       <c r="K22" s="38"/>
-      <c r="L22" s="70"/>
+      <c r="L22" s="68"/>
       <c r="M22" s="38"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
-      <c r="P22" s="72"/>
+      <c r="P22" s="70"/>
       <c r="Q22" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P22,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P22,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -17776,7 +17776,7 @@
     <row r="23" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A23" s="38"/>
       <c r="B23" s="38"/>
-      <c r="C23" s="39"/>
+      <c r="C23" s="38"/>
       <c r="D23" s="38"/>
       <c r="E23" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D23,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D23,Region!$A$1:$B$9,2,FALSE))</f>
@@ -17794,11 +17794,11 @@
       </c>
       <c r="J23" s="38"/>
       <c r="K23" s="38"/>
-      <c r="L23" s="70"/>
+      <c r="L23" s="68"/>
       <c r="M23" s="38"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
-      <c r="P23" s="72"/>
+      <c r="P23" s="70"/>
       <c r="Q23" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P23,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P23,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -17843,7 +17843,7 @@
     <row r="24" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A24" s="38"/>
       <c r="B24" s="38"/>
-      <c r="C24" s="39"/>
+      <c r="C24" s="38"/>
       <c r="D24" s="38"/>
       <c r="E24" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D24,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D24,Region!$A$1:$B$9,2,FALSE))</f>
@@ -17861,11 +17861,11 @@
       </c>
       <c r="J24" s="38"/>
       <c r="K24" s="38"/>
-      <c r="L24" s="70"/>
+      <c r="L24" s="68"/>
       <c r="M24" s="38"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
-      <c r="P24" s="72"/>
+      <c r="P24" s="70"/>
       <c r="Q24" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P24,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P24,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -17910,7 +17910,7 @@
     <row r="25" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A25" s="38"/>
       <c r="B25" s="38"/>
-      <c r="C25" s="39"/>
+      <c r="C25" s="38"/>
       <c r="D25" s="38"/>
       <c r="E25" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D25,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D25,Region!$A$1:$B$9,2,FALSE))</f>
@@ -17928,11 +17928,11 @@
       </c>
       <c r="J25" s="38"/>
       <c r="K25" s="38"/>
-      <c r="L25" s="70"/>
+      <c r="L25" s="68"/>
       <c r="M25" s="38"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
-      <c r="P25" s="72"/>
+      <c r="P25" s="70"/>
       <c r="Q25" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P25,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P25,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -17977,7 +17977,7 @@
     <row r="26" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A26" s="38"/>
       <c r="B26" s="38"/>
-      <c r="C26" s="39"/>
+      <c r="C26" s="38"/>
       <c r="D26" s="38"/>
       <c r="E26" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D26,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D26,Region!$A$1:$B$9,2,FALSE))</f>
@@ -17995,11 +17995,11 @@
       </c>
       <c r="J26" s="38"/>
       <c r="K26" s="38"/>
-      <c r="L26" s="70"/>
+      <c r="L26" s="68"/>
       <c r="M26" s="38"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
-      <c r="P26" s="72"/>
+      <c r="P26" s="70"/>
       <c r="Q26" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P26,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P26,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -18044,7 +18044,7 @@
     <row r="27" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A27" s="38"/>
       <c r="B27" s="38"/>
-      <c r="C27" s="39"/>
+      <c r="C27" s="38"/>
       <c r="D27" s="38"/>
       <c r="E27" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D27,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D27,Region!$A$1:$B$9,2,FALSE))</f>
@@ -18062,11 +18062,11 @@
       </c>
       <c r="J27" s="38"/>
       <c r="K27" s="38"/>
-      <c r="L27" s="70"/>
+      <c r="L27" s="68"/>
       <c r="M27" s="38"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
-      <c r="P27" s="72"/>
+      <c r="P27" s="70"/>
       <c r="Q27" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P27,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P27,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -18111,7 +18111,7 @@
     <row r="28" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A28" s="38"/>
       <c r="B28" s="38"/>
-      <c r="C28" s="39"/>
+      <c r="C28" s="38"/>
       <c r="D28" s="38"/>
       <c r="E28" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D28,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D28,Region!$A$1:$B$9,2,FALSE))</f>
@@ -18129,11 +18129,11 @@
       </c>
       <c r="J28" s="38"/>
       <c r="K28" s="38"/>
-      <c r="L28" s="70"/>
+      <c r="L28" s="68"/>
       <c r="M28" s="38"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
-      <c r="P28" s="72"/>
+      <c r="P28" s="70"/>
       <c r="Q28" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P28,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P28,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -18178,7 +18178,7 @@
     <row r="29" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A29" s="38"/>
       <c r="B29" s="38"/>
-      <c r="C29" s="39"/>
+      <c r="C29" s="38"/>
       <c r="D29" s="38"/>
       <c r="E29" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D29,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D29,Region!$A$1:$B$9,2,FALSE))</f>
@@ -18196,11 +18196,11 @@
       </c>
       <c r="J29" s="38"/>
       <c r="K29" s="38"/>
-      <c r="L29" s="70"/>
+      <c r="L29" s="68"/>
       <c r="M29" s="38"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
-      <c r="P29" s="72"/>
+      <c r="P29" s="70"/>
       <c r="Q29" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P29,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P29,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -18245,7 +18245,7 @@
     <row r="30" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A30" s="38"/>
       <c r="B30" s="38"/>
-      <c r="C30" s="39"/>
+      <c r="C30" s="38"/>
       <c r="D30" s="38"/>
       <c r="E30" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D30,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D30,Region!$A$1:$B$9,2,FALSE))</f>
@@ -18263,11 +18263,11 @@
       </c>
       <c r="J30" s="38"/>
       <c r="K30" s="38"/>
-      <c r="L30" s="70"/>
+      <c r="L30" s="68"/>
       <c r="M30" s="38"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
-      <c r="P30" s="72"/>
+      <c r="P30" s="70"/>
       <c r="Q30" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P30,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P30,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -18312,7 +18312,7 @@
     <row r="31" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A31" s="38"/>
       <c r="B31" s="38"/>
-      <c r="C31" s="39"/>
+      <c r="C31" s="38"/>
       <c r="D31" s="38"/>
       <c r="E31" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D31,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D31,Region!$A$1:$B$9,2,FALSE))</f>
@@ -18330,11 +18330,11 @@
       </c>
       <c r="J31" s="38"/>
       <c r="K31" s="38"/>
-      <c r="L31" s="70"/>
+      <c r="L31" s="68"/>
       <c r="M31" s="38"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
-      <c r="P31" s="72"/>
+      <c r="P31" s="70"/>
       <c r="Q31" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P31,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P31,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -18379,7 +18379,7 @@
     <row r="32" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A32" s="38"/>
       <c r="B32" s="38"/>
-      <c r="C32" s="39"/>
+      <c r="C32" s="38"/>
       <c r="D32" s="38"/>
       <c r="E32" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D32,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D32,Region!$A$1:$B$9,2,FALSE))</f>
@@ -18397,11 +18397,11 @@
       </c>
       <c r="J32" s="38"/>
       <c r="K32" s="38"/>
-      <c r="L32" s="70"/>
+      <c r="L32" s="68"/>
       <c r="M32" s="38"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
-      <c r="P32" s="72"/>
+      <c r="P32" s="70"/>
       <c r="Q32" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P32,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P32,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -18446,7 +18446,7 @@
     <row r="33" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A33" s="38"/>
       <c r="B33" s="38"/>
-      <c r="C33" s="39"/>
+      <c r="C33" s="38"/>
       <c r="D33" s="38"/>
       <c r="E33" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D33,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D33,Region!$A$1:$B$9,2,FALSE))</f>
@@ -18464,11 +18464,11 @@
       </c>
       <c r="J33" s="38"/>
       <c r="K33" s="38"/>
-      <c r="L33" s="70"/>
+      <c r="L33" s="68"/>
       <c r="M33" s="38"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
-      <c r="P33" s="72"/>
+      <c r="P33" s="70"/>
       <c r="Q33" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P33,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P33,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -18513,7 +18513,7 @@
     <row r="34" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A34" s="38"/>
       <c r="B34" s="38"/>
-      <c r="C34" s="39"/>
+      <c r="C34" s="38"/>
       <c r="D34" s="38"/>
       <c r="E34" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D34,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D34,Region!$A$1:$B$9,2,FALSE))</f>
@@ -18531,11 +18531,11 @@
       </c>
       <c r="J34" s="38"/>
       <c r="K34" s="38"/>
-      <c r="L34" s="70"/>
+      <c r="L34" s="68"/>
       <c r="M34" s="38"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
-      <c r="P34" s="72"/>
+      <c r="P34" s="70"/>
       <c r="Q34" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P34,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P34,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -18580,7 +18580,7 @@
     <row r="35" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A35" s="38"/>
       <c r="B35" s="38"/>
-      <c r="C35" s="39"/>
+      <c r="C35" s="38"/>
       <c r="D35" s="38"/>
       <c r="E35" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D35,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D35,Region!$A$1:$B$9,2,FALSE))</f>
@@ -18598,11 +18598,11 @@
       </c>
       <c r="J35" s="38"/>
       <c r="K35" s="38"/>
-      <c r="L35" s="70"/>
+      <c r="L35" s="68"/>
       <c r="M35" s="38"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
-      <c r="P35" s="72"/>
+      <c r="P35" s="70"/>
       <c r="Q35" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P35,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P35,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -18647,7 +18647,7 @@
     <row r="36" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A36" s="38"/>
       <c r="B36" s="38"/>
-      <c r="C36" s="39"/>
+      <c r="C36" s="38"/>
       <c r="D36" s="38"/>
       <c r="E36" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D36,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D36,Region!$A$1:$B$9,2,FALSE))</f>
@@ -18665,11 +18665,11 @@
       </c>
       <c r="J36" s="38"/>
       <c r="K36" s="38"/>
-      <c r="L36" s="70"/>
+      <c r="L36" s="68"/>
       <c r="M36" s="38"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
-      <c r="P36" s="72"/>
+      <c r="P36" s="70"/>
       <c r="Q36" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P36,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P36,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -18714,7 +18714,7 @@
     <row r="37" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A37" s="38"/>
       <c r="B37" s="38"/>
-      <c r="C37" s="39"/>
+      <c r="C37" s="38"/>
       <c r="D37" s="38"/>
       <c r="E37" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D37,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D37,Region!$A$1:$B$9,2,FALSE))</f>
@@ -18732,11 +18732,11 @@
       </c>
       <c r="J37" s="38"/>
       <c r="K37" s="38"/>
-      <c r="L37" s="70"/>
+      <c r="L37" s="68"/>
       <c r="M37" s="38"/>
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
-      <c r="P37" s="72"/>
+      <c r="P37" s="70"/>
       <c r="Q37" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P37,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P37,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -18781,7 +18781,7 @@
     <row r="38" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A38" s="38"/>
       <c r="B38" s="38"/>
-      <c r="C38" s="39"/>
+      <c r="C38" s="38"/>
       <c r="D38" s="38"/>
       <c r="E38" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D38,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D38,Region!$A$1:$B$9,2,FALSE))</f>
@@ -18799,11 +18799,11 @@
       </c>
       <c r="J38" s="38"/>
       <c r="K38" s="38"/>
-      <c r="L38" s="70"/>
+      <c r="L38" s="68"/>
       <c r="M38" s="38"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
-      <c r="P38" s="72"/>
+      <c r="P38" s="70"/>
       <c r="Q38" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P38,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P38,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -18848,7 +18848,7 @@
     <row r="39" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A39" s="38"/>
       <c r="B39" s="38"/>
-      <c r="C39" s="39"/>
+      <c r="C39" s="38"/>
       <c r="D39" s="38"/>
       <c r="E39" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D39,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D39,Region!$A$1:$B$9,2,FALSE))</f>
@@ -18866,11 +18866,11 @@
       </c>
       <c r="J39" s="38"/>
       <c r="K39" s="38"/>
-      <c r="L39" s="70"/>
+      <c r="L39" s="68"/>
       <c r="M39" s="38"/>
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
-      <c r="P39" s="72"/>
+      <c r="P39" s="70"/>
       <c r="Q39" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P39,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P39,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -18915,7 +18915,7 @@
     <row r="40" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A40" s="38"/>
       <c r="B40" s="38"/>
-      <c r="C40" s="39"/>
+      <c r="C40" s="38"/>
       <c r="D40" s="38"/>
       <c r="E40" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D40,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D40,Region!$A$1:$B$9,2,FALSE))</f>
@@ -18933,11 +18933,11 @@
       </c>
       <c r="J40" s="38"/>
       <c r="K40" s="38"/>
-      <c r="L40" s="70"/>
+      <c r="L40" s="68"/>
       <c r="M40" s="38"/>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
-      <c r="P40" s="72"/>
+      <c r="P40" s="70"/>
       <c r="Q40" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P40,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P40,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -18982,7 +18982,7 @@
     <row r="41" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A41" s="38"/>
       <c r="B41" s="38"/>
-      <c r="C41" s="39"/>
+      <c r="C41" s="38"/>
       <c r="D41" s="38"/>
       <c r="E41" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D41,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D41,Region!$A$1:$B$9,2,FALSE))</f>
@@ -19000,11 +19000,11 @@
       </c>
       <c r="J41" s="38"/>
       <c r="K41" s="38"/>
-      <c r="L41" s="70"/>
+      <c r="L41" s="68"/>
       <c r="M41" s="38"/>
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
-      <c r="P41" s="72"/>
+      <c r="P41" s="70"/>
       <c r="Q41" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P41,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P41,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -19049,7 +19049,7 @@
     <row r="42" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A42" s="38"/>
       <c r="B42" s="38"/>
-      <c r="C42" s="39"/>
+      <c r="C42" s="38"/>
       <c r="D42" s="38"/>
       <c r="E42" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D42,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D42,Region!$A$1:$B$9,2,FALSE))</f>
@@ -19067,11 +19067,11 @@
       </c>
       <c r="J42" s="38"/>
       <c r="K42" s="38"/>
-      <c r="L42" s="70"/>
+      <c r="L42" s="68"/>
       <c r="M42" s="38"/>
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
-      <c r="P42" s="72"/>
+      <c r="P42" s="70"/>
       <c r="Q42" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P42,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P42,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -19116,7 +19116,7 @@
     <row r="43" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A43" s="38"/>
       <c r="B43" s="38"/>
-      <c r="C43" s="39"/>
+      <c r="C43" s="38"/>
       <c r="D43" s="38"/>
       <c r="E43" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D43,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D43,Region!$A$1:$B$9,2,FALSE))</f>
@@ -19134,11 +19134,11 @@
       </c>
       <c r="J43" s="38"/>
       <c r="K43" s="38"/>
-      <c r="L43" s="70"/>
+      <c r="L43" s="68"/>
       <c r="M43" s="38"/>
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
-      <c r="P43" s="72"/>
+      <c r="P43" s="70"/>
       <c r="Q43" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P43,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P43,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -19183,7 +19183,7 @@
     <row r="44" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A44" s="38"/>
       <c r="B44" s="38"/>
-      <c r="C44" s="39"/>
+      <c r="C44" s="38"/>
       <c r="D44" s="38"/>
       <c r="E44" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D44,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D44,Region!$A$1:$B$9,2,FALSE))</f>
@@ -19201,11 +19201,11 @@
       </c>
       <c r="J44" s="38"/>
       <c r="K44" s="38"/>
-      <c r="L44" s="70"/>
+      <c r="L44" s="68"/>
       <c r="M44" s="38"/>
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
-      <c r="P44" s="72"/>
+      <c r="P44" s="70"/>
       <c r="Q44" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P44,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P44,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -19250,7 +19250,7 @@
     <row r="45" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A45" s="38"/>
       <c r="B45" s="38"/>
-      <c r="C45" s="39"/>
+      <c r="C45" s="38"/>
       <c r="D45" s="38"/>
       <c r="E45" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D45,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D45,Region!$A$1:$B$9,2,FALSE))</f>
@@ -19268,11 +19268,11 @@
       </c>
       <c r="J45" s="38"/>
       <c r="K45" s="38"/>
-      <c r="L45" s="70"/>
+      <c r="L45" s="68"/>
       <c r="M45" s="38"/>
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
-      <c r="P45" s="72"/>
+      <c r="P45" s="70"/>
       <c r="Q45" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P45,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P45,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -19317,7 +19317,7 @@
     <row r="46" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A46" s="38"/>
       <c r="B46" s="38"/>
-      <c r="C46" s="39"/>
+      <c r="C46" s="38"/>
       <c r="D46" s="38"/>
       <c r="E46" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D46,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D46,Region!$A$1:$B$9,2,FALSE))</f>
@@ -19335,11 +19335,11 @@
       </c>
       <c r="J46" s="38"/>
       <c r="K46" s="38"/>
-      <c r="L46" s="70"/>
+      <c r="L46" s="68"/>
       <c r="M46" s="38"/>
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
-      <c r="P46" s="72"/>
+      <c r="P46" s="70"/>
       <c r="Q46" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P46,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P46,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -19384,7 +19384,7 @@
     <row r="47" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A47" s="38"/>
       <c r="B47" s="38"/>
-      <c r="C47" s="39"/>
+      <c r="C47" s="38"/>
       <c r="D47" s="38"/>
       <c r="E47" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D47,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D47,Region!$A$1:$B$9,2,FALSE))</f>
@@ -19402,11 +19402,11 @@
       </c>
       <c r="J47" s="38"/>
       <c r="K47" s="38"/>
-      <c r="L47" s="70"/>
+      <c r="L47" s="68"/>
       <c r="M47" s="38"/>
       <c r="N47" s="1"/>
       <c r="O47" s="1"/>
-      <c r="P47" s="72"/>
+      <c r="P47" s="70"/>
       <c r="Q47" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P47,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P47,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -19451,7 +19451,7 @@
     <row r="48" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A48" s="38"/>
       <c r="B48" s="38"/>
-      <c r="C48" s="39"/>
+      <c r="C48" s="38"/>
       <c r="D48" s="38"/>
       <c r="E48" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D48,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D48,Region!$A$1:$B$9,2,FALSE))</f>
@@ -19469,11 +19469,11 @@
       </c>
       <c r="J48" s="38"/>
       <c r="K48" s="38"/>
-      <c r="L48" s="70"/>
+      <c r="L48" s="68"/>
       <c r="M48" s="38"/>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
-      <c r="P48" s="72"/>
+      <c r="P48" s="70"/>
       <c r="Q48" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P48,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P48,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -19518,7 +19518,7 @@
     <row r="49" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A49" s="38"/>
       <c r="B49" s="38"/>
-      <c r="C49" s="39"/>
+      <c r="C49" s="38"/>
       <c r="D49" s="38"/>
       <c r="E49" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D49,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D49,Region!$A$1:$B$9,2,FALSE))</f>
@@ -19536,11 +19536,11 @@
       </c>
       <c r="J49" s="38"/>
       <c r="K49" s="38"/>
-      <c r="L49" s="70"/>
+      <c r="L49" s="68"/>
       <c r="M49" s="38"/>
       <c r="N49" s="1"/>
       <c r="O49" s="1"/>
-      <c r="P49" s="72"/>
+      <c r="P49" s="70"/>
       <c r="Q49" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P49,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P49,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -19585,7 +19585,7 @@
     <row r="50" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A50" s="38"/>
       <c r="B50" s="38"/>
-      <c r="C50" s="39"/>
+      <c r="C50" s="38"/>
       <c r="D50" s="38"/>
       <c r="E50" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D50,Region!$A$1:$B$9,2, FALSE)),"",VLOOKUP(D50,Region!$A$1:$B$9,2,FALSE))</f>
@@ -19603,11 +19603,11 @@
       </c>
       <c r="J50" s="38"/>
       <c r="K50" s="38"/>
-      <c r="L50" s="70"/>
+      <c r="L50" s="68"/>
       <c r="M50" s="38"/>
       <c r="N50" s="1"/>
       <c r="O50" s="1"/>
-      <c r="P50" s="72"/>
+      <c r="P50" s="70"/>
       <c r="Q50" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P50,Services!$A$1:$B$45,2,FALSE)),"",VLOOKUP(P50,Services!$A$1:$B$45,2,FALSE))</f>
         <v/>
@@ -19649,19 +19649,279 @@
       </c>
       <c r="AF50" s="38"/>
     </row>
-    <row r="51" spans="1:32" s="40" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" spans="1:32" s="40" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" spans="1:32" s="40" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" spans="1:32" s="40" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="55" spans="1:32" s="40" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="56" spans="1:32" s="40" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="57" spans="1:32" s="40" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="58" spans="1:32" s="40" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="59" spans="1:32" s="40" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="60" spans="1:32" s="40" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="61" spans="1:32" s="40" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="62" spans="1:32" s="40" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="63" spans="1:32" s="40" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A51"/>
+      <c r="B51"/>
+      <c r="C51"/>
+      <c r="D51"/>
+      <c r="F51"/>
+      <c r="H51"/>
+      <c r="J51"/>
+      <c r="K51"/>
+      <c r="L51"/>
+      <c r="M51"/>
+      <c r="P51"/>
+      <c r="R51"/>
+      <c r="T51"/>
+      <c r="V51"/>
+      <c r="X51"/>
+      <c r="Z51"/>
+      <c r="AB51"/>
+      <c r="AD51"/>
+      <c r="AF51"/>
+    </row>
+    <row r="52" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A52"/>
+      <c r="B52"/>
+      <c r="C52"/>
+      <c r="D52"/>
+      <c r="F52"/>
+      <c r="H52"/>
+      <c r="J52"/>
+      <c r="K52"/>
+      <c r="L52"/>
+      <c r="M52"/>
+      <c r="P52"/>
+      <c r="R52"/>
+      <c r="T52"/>
+      <c r="V52"/>
+      <c r="X52"/>
+      <c r="Z52"/>
+      <c r="AB52"/>
+      <c r="AD52"/>
+      <c r="AF52"/>
+    </row>
+    <row r="53" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A53"/>
+      <c r="B53"/>
+      <c r="C53"/>
+      <c r="D53"/>
+      <c r="F53"/>
+      <c r="H53"/>
+      <c r="J53"/>
+      <c r="K53"/>
+      <c r="L53"/>
+      <c r="M53"/>
+      <c r="P53"/>
+      <c r="R53"/>
+      <c r="T53"/>
+      <c r="V53"/>
+      <c r="X53"/>
+      <c r="Z53"/>
+      <c r="AB53"/>
+      <c r="AD53"/>
+      <c r="AF53"/>
+    </row>
+    <row r="54" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A54"/>
+      <c r="B54"/>
+      <c r="C54"/>
+      <c r="D54"/>
+      <c r="F54"/>
+      <c r="H54"/>
+      <c r="J54"/>
+      <c r="K54"/>
+      <c r="L54"/>
+      <c r="M54"/>
+      <c r="P54"/>
+      <c r="R54"/>
+      <c r="T54"/>
+      <c r="V54"/>
+      <c r="X54"/>
+      <c r="Z54"/>
+      <c r="AB54"/>
+      <c r="AD54"/>
+      <c r="AF54"/>
+    </row>
+    <row r="55" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A55"/>
+      <c r="B55"/>
+      <c r="C55"/>
+      <c r="D55"/>
+      <c r="F55"/>
+      <c r="H55"/>
+      <c r="J55"/>
+      <c r="K55"/>
+      <c r="L55"/>
+      <c r="M55"/>
+      <c r="P55"/>
+      <c r="R55"/>
+      <c r="T55"/>
+      <c r="V55"/>
+      <c r="X55"/>
+      <c r="Z55"/>
+      <c r="AB55"/>
+      <c r="AD55"/>
+      <c r="AF55"/>
+    </row>
+    <row r="56" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A56"/>
+      <c r="B56"/>
+      <c r="C56"/>
+      <c r="D56"/>
+      <c r="F56"/>
+      <c r="H56"/>
+      <c r="J56"/>
+      <c r="K56"/>
+      <c r="L56"/>
+      <c r="M56"/>
+      <c r="P56"/>
+      <c r="R56"/>
+      <c r="T56"/>
+      <c r="V56"/>
+      <c r="X56"/>
+      <c r="Z56"/>
+      <c r="AB56"/>
+      <c r="AD56"/>
+      <c r="AF56"/>
+    </row>
+    <row r="57" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A57"/>
+      <c r="B57"/>
+      <c r="C57"/>
+      <c r="D57"/>
+      <c r="F57"/>
+      <c r="H57"/>
+      <c r="J57"/>
+      <c r="K57"/>
+      <c r="L57"/>
+      <c r="M57"/>
+      <c r="P57"/>
+      <c r="R57"/>
+      <c r="T57"/>
+      <c r="V57"/>
+      <c r="X57"/>
+      <c r="Z57"/>
+      <c r="AB57"/>
+      <c r="AD57"/>
+      <c r="AF57"/>
+    </row>
+    <row r="58" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A58"/>
+      <c r="B58"/>
+      <c r="C58"/>
+      <c r="D58"/>
+      <c r="F58"/>
+      <c r="H58"/>
+      <c r="J58"/>
+      <c r="K58"/>
+      <c r="L58"/>
+      <c r="M58"/>
+      <c r="P58"/>
+      <c r="R58"/>
+      <c r="T58"/>
+      <c r="V58"/>
+      <c r="X58"/>
+      <c r="Z58"/>
+      <c r="AB58"/>
+      <c r="AD58"/>
+      <c r="AF58"/>
+    </row>
+    <row r="59" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A59"/>
+      <c r="B59"/>
+      <c r="C59"/>
+      <c r="D59"/>
+      <c r="F59"/>
+      <c r="H59"/>
+      <c r="J59"/>
+      <c r="K59"/>
+      <c r="L59"/>
+      <c r="M59"/>
+      <c r="P59"/>
+      <c r="R59"/>
+      <c r="T59"/>
+      <c r="V59"/>
+      <c r="X59"/>
+      <c r="Z59"/>
+      <c r="AB59"/>
+      <c r="AD59"/>
+      <c r="AF59"/>
+    </row>
+    <row r="60" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A60"/>
+      <c r="B60"/>
+      <c r="C60"/>
+      <c r="D60"/>
+      <c r="F60"/>
+      <c r="H60"/>
+      <c r="J60"/>
+      <c r="K60"/>
+      <c r="L60"/>
+      <c r="M60"/>
+      <c r="P60"/>
+      <c r="R60"/>
+      <c r="T60"/>
+      <c r="V60"/>
+      <c r="X60"/>
+      <c r="Z60"/>
+      <c r="AB60"/>
+      <c r="AD60"/>
+      <c r="AF60"/>
+    </row>
+    <row r="61" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A61"/>
+      <c r="B61"/>
+      <c r="C61"/>
+      <c r="D61"/>
+      <c r="F61"/>
+      <c r="H61"/>
+      <c r="J61"/>
+      <c r="K61"/>
+      <c r="L61"/>
+      <c r="M61"/>
+      <c r="P61"/>
+      <c r="R61"/>
+      <c r="T61"/>
+      <c r="V61"/>
+      <c r="X61"/>
+      <c r="Z61"/>
+      <c r="AB61"/>
+      <c r="AD61"/>
+      <c r="AF61"/>
+    </row>
+    <row r="62" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A62"/>
+      <c r="B62"/>
+      <c r="C62"/>
+      <c r="D62"/>
+      <c r="F62"/>
+      <c r="H62"/>
+      <c r="J62"/>
+      <c r="K62"/>
+      <c r="L62"/>
+      <c r="M62"/>
+      <c r="P62"/>
+      <c r="R62"/>
+      <c r="T62"/>
+      <c r="V62"/>
+      <c r="X62"/>
+      <c r="Z62"/>
+      <c r="AB62"/>
+      <c r="AD62"/>
+      <c r="AF62"/>
+    </row>
+    <row r="63" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A63"/>
+      <c r="B63"/>
+      <c r="C63"/>
+      <c r="D63"/>
+      <c r="F63"/>
+      <c r="H63"/>
+      <c r="J63"/>
+      <c r="K63"/>
+      <c r="L63"/>
+      <c r="M63"/>
+      <c r="P63"/>
+      <c r="R63"/>
+      <c r="T63"/>
+      <c r="V63"/>
+      <c r="X63"/>
+      <c r="Z63"/>
+      <c r="AB63"/>
+      <c r="AD63"/>
+      <c r="AF63"/>
+    </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <phoneticPr fontId="8" type="noConversion"/>
@@ -19738,7 +19998,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1185</v>
+        <v>1262</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -27480,122 +27740,122 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="74" t="s">
-        <v>1262</v>
-      </c>
-      <c r="B1" s="75">
+      <c r="A1" s="72" t="s">
+        <v>1261</v>
+      </c>
+      <c r="B1" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="76" t="s">
-        <v>1261</v>
-      </c>
-      <c r="B2" s="75">
+      <c r="A2" s="74" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B2" s="73">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="74" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B3" s="73">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="74" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B4" s="73">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="74" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B5" s="73">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="74" t="s">
         <v>1251</v>
       </c>
-      <c r="B3" s="75">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="76" t="s">
-        <v>1248</v>
-      </c>
-      <c r="B4" s="75">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="76" t="s">
+      <c r="B6" s="73">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="74" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B7" s="73">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="74" t="s">
+        <v>1253</v>
+      </c>
+      <c r="B8" s="73">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="74" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B9" s="73">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="74" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B10" s="73">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="74" t="s">
         <v>1249</v>
       </c>
-      <c r="B5" s="75">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="76" t="s">
-        <v>1252</v>
-      </c>
-      <c r="B6" s="75">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="76" t="s">
-        <v>1253</v>
-      </c>
-      <c r="B7" s="75">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="76" t="s">
-        <v>1254</v>
-      </c>
-      <c r="B8" s="75">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="76" t="s">
-        <v>1255</v>
-      </c>
-      <c r="B9" s="75">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="76" t="s">
+      <c r="B11" s="73">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="74" t="s">
         <v>1256</v>
       </c>
-      <c r="B10" s="75">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="76" t="s">
-        <v>1250</v>
-      </c>
-      <c r="B11" s="75">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="76" t="s">
+      <c r="B12" s="73">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="74" t="s">
         <v>1257</v>
       </c>
-      <c r="B12" s="75">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="76" t="s">
+      <c r="B13" s="73">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="74" t="s">
         <v>1258</v>
       </c>
-      <c r="B13" s="75">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="76" t="s">
+      <c r="B14" s="73">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="74" t="s">
         <v>1259</v>
       </c>
-      <c r="B14" s="75">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="76" t="s">
-        <v>1260</v>
-      </c>
-      <c r="B15" s="75">
+      <c r="B15" s="73">
         <v>15</v>
       </c>
     </row>

</xml_diff>